<commit_message>
Prevented "Serial" from reflecting "Ordinal End" as being lower than the "Ordinal Start"
</commit_message>
<xml_diff>
--- a/math-decks/basic-arithmetic-number-sense/Card Types/{Data Sheet Chunk} 1. Addition and Subtraction.xlsx
+++ b/math-decks/basic-arithmetic-number-sense/Card Types/{Data Sheet Chunk} 1. Addition and Subtraction.xlsx
@@ -148,7 +148,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0070C0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF0070C0"/>
@@ -185,8 +195,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="Table Style 1" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="3"/>
-      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -561,7 +571,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>IF(ISNUMBER(C3),"arith_" &amp; INDEX(Operations[],J3,2) &amp; "_g" &amp; TEXT(C3, "00") &amp; "_" &amp; TEXT(D3, "00") &amp; "_o" &amp; TEXT(E3, "00") &amp; IF(AND(ISNUMBER(F3), F3&lt;&gt;E3), "_" &amp; TEXT(F3, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C3),"arith_" &amp; INDEX(Operations[],J3,2) &amp; "_g" &amp; TEXT(C3, "00") &amp; "_" &amp; TEXT(D3, "00") &amp; "_o" &amp; TEXT(E3, "00") &amp; IF(AND(ISNUMBER(F3), F3&gt;E3), "_" &amp; TEXT(F3, "00"), ""), "")</f>
         <v>arith_add_g01_00_o01_02</v>
       </c>
       <c r="B3" t="str">
@@ -601,7 +611,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>IF(ISNUMBER(C4),"arith_" &amp; INDEX(Operations[],J4,2) &amp; "_g" &amp; TEXT(C4, "00") &amp; "_" &amp; TEXT(D4, "00") &amp; "_o" &amp; TEXT(E4, "00") &amp; IF(AND(ISNUMBER(F4), F4&lt;&gt;E4), "_" &amp; TEXT(F4, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C4),"arith_" &amp; INDEX(Operations[],J4,2) &amp; "_g" &amp; TEXT(C4, "00") &amp; "_" &amp; TEXT(D4, "00") &amp; "_o" &amp; TEXT(E4, "00") &amp; IF(AND(ISNUMBER(F4), F4&gt;E4), "_" &amp; TEXT(F4, "00"), ""), "")</f>
         <v>arith_add_g01_00_o02_03</v>
       </c>
       <c r="B4" t="str">
@@ -640,7 +650,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>IF(ISNUMBER(C5),"arith_" &amp; INDEX(Operations[],J5,2) &amp; "_g" &amp; TEXT(C5, "00") &amp; "_" &amp; TEXT(D5, "00") &amp; "_o" &amp; TEXT(E5, "00") &amp; IF(AND(ISNUMBER(F5), F5&lt;&gt;E5), "_" &amp; TEXT(F5, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C5),"arith_" &amp; INDEX(Operations[],J5,2) &amp; "_g" &amp; TEXT(C5, "00") &amp; "_" &amp; TEXT(D5, "00") &amp; "_o" &amp; TEXT(E5, "00") &amp; IF(AND(ISNUMBER(F5), F5&gt;E5), "_" &amp; TEXT(F5, "00"), ""), "")</f>
         <v>arith_add_g01_00_o03_04</v>
       </c>
       <c r="B5" t="str">
@@ -673,7 +683,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>IF(ISNUMBER(C6),"arith_" &amp; INDEX(Operations[],J6,2) &amp; "_g" &amp; TEXT(C6, "00") &amp; "_" &amp; TEXT(D6, "00") &amp; "_o" &amp; TEXT(E6, "00") &amp; IF(AND(ISNUMBER(F6), F6&lt;&gt;E6), "_" &amp; TEXT(F6, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C6),"arith_" &amp; INDEX(Operations[],J6,2) &amp; "_g" &amp; TEXT(C6, "00") &amp; "_" &amp; TEXT(D6, "00") &amp; "_o" &amp; TEXT(E6, "00") &amp; IF(AND(ISNUMBER(F6), F6&gt;E6), "_" &amp; TEXT(F6, "00"), ""), "")</f>
         <v>arith_add_g01_00_o04_05</v>
       </c>
       <c r="B6" t="str">
@@ -712,7 +722,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>IF(ISNUMBER(C7),"arith_" &amp; INDEX(Operations[],J7,2) &amp; "_g" &amp; TEXT(C7, "00") &amp; "_" &amp; TEXT(D7, "00") &amp; "_o" &amp; TEXT(E7, "00") &amp; IF(AND(ISNUMBER(F7), F7&lt;&gt;E7), "_" &amp; TEXT(F7, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C7),"arith_" &amp; INDEX(Operations[],J7,2) &amp; "_g" &amp; TEXT(C7, "00") &amp; "_" &amp; TEXT(D7, "00") &amp; "_o" &amp; TEXT(E7, "00") &amp; IF(AND(ISNUMBER(F7), F7&gt;E7), "_" &amp; TEXT(F7, "00"), ""), "")</f>
         <v>arith_add_g01_00_o05_06</v>
       </c>
       <c r="B7" t="str">
@@ -751,7 +761,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>IF(ISNUMBER(C8),"arith_" &amp; INDEX(Operations[],J8,2) &amp; "_g" &amp; TEXT(C8, "00") &amp; "_" &amp; TEXT(D8, "00") &amp; "_o" &amp; TEXT(E8, "00") &amp; IF(AND(ISNUMBER(F8), F8&lt;&gt;E8), "_" &amp; TEXT(F8, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C8),"arith_" &amp; INDEX(Operations[],J8,2) &amp; "_g" &amp; TEXT(C8, "00") &amp; "_" &amp; TEXT(D8, "00") &amp; "_o" &amp; TEXT(E8, "00") &amp; IF(AND(ISNUMBER(F8), F8&gt;E8), "_" &amp; TEXT(F8, "00"), ""), "")</f>
         <v>arith_add_g01_00_o06_07</v>
       </c>
       <c r="B8" t="str">
@@ -790,7 +800,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>IF(ISNUMBER(C9),"arith_" &amp; INDEX(Operations[],J9,2) &amp; "_g" &amp; TEXT(C9, "00") &amp; "_" &amp; TEXT(D9, "00") &amp; "_o" &amp; TEXT(E9, "00") &amp; IF(AND(ISNUMBER(F9), F9&lt;&gt;E9), "_" &amp; TEXT(F9, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C9),"arith_" &amp; INDEX(Operations[],J9,2) &amp; "_g" &amp; TEXT(C9, "00") &amp; "_" &amp; TEXT(D9, "00") &amp; "_o" &amp; TEXT(E9, "00") &amp; IF(AND(ISNUMBER(F9), F9&gt;E9), "_" &amp; TEXT(F9, "00"), ""), "")</f>
         <v>arith_add_g01_00_o07_08</v>
       </c>
       <c r="B9" t="str">
@@ -823,7 +833,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>IF(ISNUMBER(C10),"arith_" &amp; INDEX(Operations[],J10,2) &amp; "_g" &amp; TEXT(C10, "00") &amp; "_" &amp; TEXT(D10, "00") &amp; "_o" &amp; TEXT(E10, "00") &amp; IF(AND(ISNUMBER(F10), F10&lt;&gt;E10), "_" &amp; TEXT(F10, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C10),"arith_" &amp; INDEX(Operations[],J10,2) &amp; "_g" &amp; TEXT(C10, "00") &amp; "_" &amp; TEXT(D10, "00") &amp; "_o" &amp; TEXT(E10, "00") &amp; IF(AND(ISNUMBER(F10), F10&gt;E10), "_" &amp; TEXT(F10, "00"), ""), "")</f>
         <v>arith_add_g01_00_o08_09</v>
       </c>
       <c r="B10" t="str">
@@ -856,7 +866,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>IF(ISNUMBER(C11),"arith_" &amp; INDEX(Operations[],J11,2) &amp; "_g" &amp; TEXT(C11, "00") &amp; "_" &amp; TEXT(D11, "00") &amp; "_o" &amp; TEXT(E11, "00") &amp; IF(AND(ISNUMBER(F11), F11&lt;&gt;E11), "_" &amp; TEXT(F11, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C11),"arith_" &amp; INDEX(Operations[],J11,2) &amp; "_g" &amp; TEXT(C11, "00") &amp; "_" &amp; TEXT(D11, "00") &amp; "_o" &amp; TEXT(E11, "00") &amp; IF(AND(ISNUMBER(F11), F11&gt;E11), "_" &amp; TEXT(F11, "00"), ""), "")</f>
         <v>arith_add_g01_00_o09_10</v>
       </c>
       <c r="B11" t="str">
@@ -889,7 +899,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>IF(ISNUMBER(C12),"arith_" &amp; INDEX(Operations[],J12,2) &amp; "_g" &amp; TEXT(C12, "00") &amp; "_" &amp; TEXT(D12, "00") &amp; "_o" &amp; TEXT(E12, "00") &amp; IF(AND(ISNUMBER(F12), F12&lt;&gt;E12), "_" &amp; TEXT(F12, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C12),"arith_" &amp; INDEX(Operations[],J12,2) &amp; "_g" &amp; TEXT(C12, "00") &amp; "_" &amp; TEXT(D12, "00") &amp; "_o" &amp; TEXT(E12, "00") &amp; IF(AND(ISNUMBER(F12), F12&gt;E12), "_" &amp; TEXT(F12, "00"), ""), "")</f>
         <v>arith_add_g01_00_o10</v>
       </c>
       <c r="B12" t="str">
@@ -919,7 +929,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>IF(ISNUMBER(C13),"arith_" &amp; INDEX(Operations[],J13,2) &amp; "_g" &amp; TEXT(C13, "00") &amp; "_" &amp; TEXT(D13, "00") &amp; "_o" &amp; TEXT(E13, "00") &amp; IF(AND(ISNUMBER(F13), F13&lt;&gt;E13), "_" &amp; TEXT(F13, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C13),"arith_" &amp; INDEX(Operations[],J13,2) &amp; "_g" &amp; TEXT(C13, "00") &amp; "_" &amp; TEXT(D13, "00") &amp; "_o" &amp; TEXT(E13, "00") &amp; IF(AND(ISNUMBER(F13), F13&gt;E13), "_" &amp; TEXT(F13, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B13" t="str">
@@ -948,7 +958,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>IF(ISNUMBER(C14),"arith_" &amp; INDEX(Operations[],J14,2) &amp; "_g" &amp; TEXT(C14, "00") &amp; "_" &amp; TEXT(D14, "00") &amp; "_o" &amp; TEXT(E14, "00") &amp; IF(AND(ISNUMBER(F14), F14&lt;&gt;E14), "_" &amp; TEXT(F14, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C14),"arith_" &amp; INDEX(Operations[],J14,2) &amp; "_g" &amp; TEXT(C14, "00") &amp; "_" &amp; TEXT(D14, "00") &amp; "_o" &amp; TEXT(E14, "00") &amp; IF(AND(ISNUMBER(F14), F14&gt;E14), "_" &amp; TEXT(F14, "00"), ""), "")</f>
         <v>arith_add_g02_00_o01_02</v>
       </c>
       <c r="B14" t="str">
@@ -990,7 +1000,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>IF(ISNUMBER(C15),"arith_" &amp; INDEX(Operations[],J15,2) &amp; "_g" &amp; TEXT(C15, "00") &amp; "_" &amp; TEXT(D15, "00") &amp; "_o" &amp; TEXT(E15, "00") &amp; IF(AND(ISNUMBER(F15), F15&lt;&gt;E15), "_" &amp; TEXT(F15, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C15),"arith_" &amp; INDEX(Operations[],J15,2) &amp; "_g" &amp; TEXT(C15, "00") &amp; "_" &amp; TEXT(D15, "00") &amp; "_o" &amp; TEXT(E15, "00") &amp; IF(AND(ISNUMBER(F15), F15&gt;E15), "_" &amp; TEXT(F15, "00"), ""), "")</f>
         <v>arith_add_g02_00_o02_03</v>
       </c>
       <c r="B15" t="str">
@@ -1032,7 +1042,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>IF(ISNUMBER(C16),"arith_" &amp; INDEX(Operations[],J16,2) &amp; "_g" &amp; TEXT(C16, "00") &amp; "_" &amp; TEXT(D16, "00") &amp; "_o" &amp; TEXT(E16, "00") &amp; IF(AND(ISNUMBER(F16), F16&lt;&gt;E16), "_" &amp; TEXT(F16, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C16),"arith_" &amp; INDEX(Operations[],J16,2) &amp; "_g" &amp; TEXT(C16, "00") &amp; "_" &amp; TEXT(D16, "00") &amp; "_o" &amp; TEXT(E16, "00") &amp; IF(AND(ISNUMBER(F16), F16&gt;E16), "_" &amp; TEXT(F16, "00"), ""), "")</f>
         <v>arith_add_g02_00_o03_04</v>
       </c>
       <c r="B16" t="str">
@@ -1074,7 +1084,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>IF(ISNUMBER(C17),"arith_" &amp; INDEX(Operations[],J17,2) &amp; "_g" &amp; TEXT(C17, "00") &amp; "_" &amp; TEXT(D17, "00") &amp; "_o" &amp; TEXT(E17, "00") &amp; IF(AND(ISNUMBER(F17), F17&lt;&gt;E17), "_" &amp; TEXT(F17, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C17),"arith_" &amp; INDEX(Operations[],J17,2) &amp; "_g" &amp; TEXT(C17, "00") &amp; "_" &amp; TEXT(D17, "00") &amp; "_o" &amp; TEXT(E17, "00") &amp; IF(AND(ISNUMBER(F17), F17&gt;E17), "_" &amp; TEXT(F17, "00"), ""), "")</f>
         <v>arith_add_g02_00_o04_05</v>
       </c>
       <c r="B17" t="str">
@@ -1116,7 +1126,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>IF(ISNUMBER(C18),"arith_" &amp; INDEX(Operations[],J18,2) &amp; "_g" &amp; TEXT(C18, "00") &amp; "_" &amp; TEXT(D18, "00") &amp; "_o" &amp; TEXT(E18, "00") &amp; IF(AND(ISNUMBER(F18), F18&lt;&gt;E18), "_" &amp; TEXT(F18, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C18),"arith_" &amp; INDEX(Operations[],J18,2) &amp; "_g" &amp; TEXT(C18, "00") &amp; "_" &amp; TEXT(D18, "00") &amp; "_o" &amp; TEXT(E18, "00") &amp; IF(AND(ISNUMBER(F18), F18&gt;E18), "_" &amp; TEXT(F18, "00"), ""), "")</f>
         <v>arith_add_g02_00_o05_06</v>
       </c>
       <c r="B18" t="str">
@@ -1158,7 +1168,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>IF(ISNUMBER(C19),"arith_" &amp; INDEX(Operations[],J19,2) &amp; "_g" &amp; TEXT(C19, "00") &amp; "_" &amp; TEXT(D19, "00") &amp; "_o" &amp; TEXT(E19, "00") &amp; IF(AND(ISNUMBER(F19), F19&lt;&gt;E19), "_" &amp; TEXT(F19, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C19),"arith_" &amp; INDEX(Operations[],J19,2) &amp; "_g" &amp; TEXT(C19, "00") &amp; "_" &amp; TEXT(D19, "00") &amp; "_o" &amp; TEXT(E19, "00") &amp; IF(AND(ISNUMBER(F19), F19&gt;E19), "_" &amp; TEXT(F19, "00"), ""), "")</f>
         <v>arith_add_g02_00_o06_07</v>
       </c>
       <c r="B19" t="str">
@@ -1200,7 +1210,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>IF(ISNUMBER(C20),"arith_" &amp; INDEX(Operations[],J20,2) &amp; "_g" &amp; TEXT(C20, "00") &amp; "_" &amp; TEXT(D20, "00") &amp; "_o" &amp; TEXT(E20, "00") &amp; IF(AND(ISNUMBER(F20), F20&lt;&gt;E20), "_" &amp; TEXT(F20, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C20),"arith_" &amp; INDEX(Operations[],J20,2) &amp; "_g" &amp; TEXT(C20, "00") &amp; "_" &amp; TEXT(D20, "00") &amp; "_o" &amp; TEXT(E20, "00") &amp; IF(AND(ISNUMBER(F20), F20&gt;E20), "_" &amp; TEXT(F20, "00"), ""), "")</f>
         <v>arith_add_g02_00_o07_08</v>
       </c>
       <c r="B20" t="str">
@@ -1242,7 +1252,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>IF(ISNUMBER(C21),"arith_" &amp; INDEX(Operations[],J21,2) &amp; "_g" &amp; TEXT(C21, "00") &amp; "_" &amp; TEXT(D21, "00") &amp; "_o" &amp; TEXT(E21, "00") &amp; IF(AND(ISNUMBER(F21), F21&lt;&gt;E21), "_" &amp; TEXT(F21, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C21),"arith_" &amp; INDEX(Operations[],J21,2) &amp; "_g" &amp; TEXT(C21, "00") &amp; "_" &amp; TEXT(D21, "00") &amp; "_o" &amp; TEXT(E21, "00") &amp; IF(AND(ISNUMBER(F21), F21&gt;E21), "_" &amp; TEXT(F21, "00"), ""), "")</f>
         <v>arith_add_g02_00_o08_09</v>
       </c>
       <c r="B21" t="str">
@@ -1284,7 +1294,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>IF(ISNUMBER(C22),"arith_" &amp; INDEX(Operations[],J22,2) &amp; "_g" &amp; TEXT(C22, "00") &amp; "_" &amp; TEXT(D22, "00") &amp; "_o" &amp; TEXT(E22, "00") &amp; IF(AND(ISNUMBER(F22), F22&lt;&gt;E22), "_" &amp; TEXT(F22, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C22),"arith_" &amp; INDEX(Operations[],J22,2) &amp; "_g" &amp; TEXT(C22, "00") &amp; "_" &amp; TEXT(D22, "00") &amp; "_o" &amp; TEXT(E22, "00") &amp; IF(AND(ISNUMBER(F22), F22&gt;E22), "_" &amp; TEXT(F22, "00"), ""), "")</f>
         <v>arith_add_g02_00_o09_10</v>
       </c>
       <c r="B22" t="str">
@@ -1326,7 +1336,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>IF(ISNUMBER(C23),"arith_" &amp; INDEX(Operations[],J23,2) &amp; "_g" &amp; TEXT(C23, "00") &amp; "_" &amp; TEXT(D23, "00") &amp; "_o" &amp; TEXT(E23, "00") &amp; IF(AND(ISNUMBER(F23), F23&lt;&gt;E23), "_" &amp; TEXT(F23, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C23),"arith_" &amp; INDEX(Operations[],J23,2) &amp; "_g" &amp; TEXT(C23, "00") &amp; "_" &amp; TEXT(D23, "00") &amp; "_o" &amp; TEXT(E23, "00") &amp; IF(AND(ISNUMBER(F23), F23&gt;E23), "_" &amp; TEXT(F23, "00"), ""), "")</f>
         <v>arith_add_g02_00_o10</v>
       </c>
       <c r="B23" t="str">
@@ -1368,7 +1378,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>IF(ISNUMBER(C24),"arith_" &amp; INDEX(Operations[],J24,2) &amp; "_g" &amp; TEXT(C24, "00") &amp; "_" &amp; TEXT(D24, "00") &amp; "_o" &amp; TEXT(E24, "00") &amp; IF(AND(ISNUMBER(F24), F24&lt;&gt;E24), "_" &amp; TEXT(F24, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C24),"arith_" &amp; INDEX(Operations[],J24,2) &amp; "_g" &amp; TEXT(C24, "00") &amp; "_" &amp; TEXT(D24, "00") &amp; "_o" &amp; TEXT(E24, "00") &amp; IF(AND(ISNUMBER(F24), F24&gt;E24), "_" &amp; TEXT(F24, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B24" t="str">
@@ -1410,7 +1420,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>IF(ISNUMBER(C25),"arith_" &amp; INDEX(Operations[],J25,2) &amp; "_g" &amp; TEXT(C25, "00") &amp; "_" &amp; TEXT(D25, "00") &amp; "_o" &amp; TEXT(E25, "00") &amp; IF(AND(ISNUMBER(F25), F25&lt;&gt;E25), "_" &amp; TEXT(F25, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C25),"arith_" &amp; INDEX(Operations[],J25,2) &amp; "_g" &amp; TEXT(C25, "00") &amp; "_" &amp; TEXT(D25, "00") &amp; "_o" &amp; TEXT(E25, "00") &amp; IF(AND(ISNUMBER(F25), F25&gt;E25), "_" &amp; TEXT(F25, "00"), ""), "")</f>
         <v>arith_add_g03_00_o01_02</v>
       </c>
       <c r="B25" t="str">
@@ -1452,7 +1462,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>IF(ISNUMBER(C26),"arith_" &amp; INDEX(Operations[],J26,2) &amp; "_g" &amp; TEXT(C26, "00") &amp; "_" &amp; TEXT(D26, "00") &amp; "_o" &amp; TEXT(E26, "00") &amp; IF(AND(ISNUMBER(F26), F26&lt;&gt;E26), "_" &amp; TEXT(F26, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C26),"arith_" &amp; INDEX(Operations[],J26,2) &amp; "_g" &amp; TEXT(C26, "00") &amp; "_" &amp; TEXT(D26, "00") &amp; "_o" &amp; TEXT(E26, "00") &amp; IF(AND(ISNUMBER(F26), F26&gt;E26), "_" &amp; TEXT(F26, "00"), ""), "")</f>
         <v>arith_add_g03_00_o02_03</v>
       </c>
       <c r="B26" t="str">
@@ -1494,7 +1504,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>IF(ISNUMBER(C27),"arith_" &amp; INDEX(Operations[],J27,2) &amp; "_g" &amp; TEXT(C27, "00") &amp; "_" &amp; TEXT(D27, "00") &amp; "_o" &amp; TEXT(E27, "00") &amp; IF(AND(ISNUMBER(F27), F27&lt;&gt;E27), "_" &amp; TEXT(F27, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C27),"arith_" &amp; INDEX(Operations[],J27,2) &amp; "_g" &amp; TEXT(C27, "00") &amp; "_" &amp; TEXT(D27, "00") &amp; "_o" &amp; TEXT(E27, "00") &amp; IF(AND(ISNUMBER(F27), F27&gt;E27), "_" &amp; TEXT(F27, "00"), ""), "")</f>
         <v>arith_add_g03_00_o03_04</v>
       </c>
       <c r="B27" t="str">
@@ -1536,7 +1546,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>IF(ISNUMBER(C28),"arith_" &amp; INDEX(Operations[],J28,2) &amp; "_g" &amp; TEXT(C28, "00") &amp; "_" &amp; TEXT(D28, "00") &amp; "_o" &amp; TEXT(E28, "00") &amp; IF(AND(ISNUMBER(F28), F28&lt;&gt;E28), "_" &amp; TEXT(F28, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C28),"arith_" &amp; INDEX(Operations[],J28,2) &amp; "_g" &amp; TEXT(C28, "00") &amp; "_" &amp; TEXT(D28, "00") &amp; "_o" &amp; TEXT(E28, "00") &amp; IF(AND(ISNUMBER(F28), F28&gt;E28), "_" &amp; TEXT(F28, "00"), ""), "")</f>
         <v>arith_add_g03_00_o04_05</v>
       </c>
       <c r="B28" t="str">
@@ -1578,7 +1588,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>IF(ISNUMBER(C29),"arith_" &amp; INDEX(Operations[],J29,2) &amp; "_g" &amp; TEXT(C29, "00") &amp; "_" &amp; TEXT(D29, "00") &amp; "_o" &amp; TEXT(E29, "00") &amp; IF(AND(ISNUMBER(F29), F29&lt;&gt;E29), "_" &amp; TEXT(F29, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C29),"arith_" &amp; INDEX(Operations[],J29,2) &amp; "_g" &amp; TEXT(C29, "00") &amp; "_" &amp; TEXT(D29, "00") &amp; "_o" &amp; TEXT(E29, "00") &amp; IF(AND(ISNUMBER(F29), F29&gt;E29), "_" &amp; TEXT(F29, "00"), ""), "")</f>
         <v>arith_add_g03_00_o05_06</v>
       </c>
       <c r="B29" t="str">
@@ -1620,7 +1630,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>IF(ISNUMBER(C30),"arith_" &amp; INDEX(Operations[],J30,2) &amp; "_g" &amp; TEXT(C30, "00") &amp; "_" &amp; TEXT(D30, "00") &amp; "_o" &amp; TEXT(E30, "00") &amp; IF(AND(ISNUMBER(F30), F30&lt;&gt;E30), "_" &amp; TEXT(F30, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C30),"arith_" &amp; INDEX(Operations[],J30,2) &amp; "_g" &amp; TEXT(C30, "00") &amp; "_" &amp; TEXT(D30, "00") &amp; "_o" &amp; TEXT(E30, "00") &amp; IF(AND(ISNUMBER(F30), F30&gt;E30), "_" &amp; TEXT(F30, "00"), ""), "")</f>
         <v>arith_add_g03_00_o06_07</v>
       </c>
       <c r="B30" t="str">
@@ -1662,7 +1672,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>IF(ISNUMBER(C31),"arith_" &amp; INDEX(Operations[],J31,2) &amp; "_g" &amp; TEXT(C31, "00") &amp; "_" &amp; TEXT(D31, "00") &amp; "_o" &amp; TEXT(E31, "00") &amp; IF(AND(ISNUMBER(F31), F31&lt;&gt;E31), "_" &amp; TEXT(F31, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C31),"arith_" &amp; INDEX(Operations[],J31,2) &amp; "_g" &amp; TEXT(C31, "00") &amp; "_" &amp; TEXT(D31, "00") &amp; "_o" &amp; TEXT(E31, "00") &amp; IF(AND(ISNUMBER(F31), F31&gt;E31), "_" &amp; TEXT(F31, "00"), ""), "")</f>
         <v>arith_add_g03_00_o07_08</v>
       </c>
       <c r="B31" t="str">
@@ -1704,7 +1714,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>IF(ISNUMBER(C32),"arith_" &amp; INDEX(Operations[],J32,2) &amp; "_g" &amp; TEXT(C32, "00") &amp; "_" &amp; TEXT(D32, "00") &amp; "_o" &amp; TEXT(E32, "00") &amp; IF(AND(ISNUMBER(F32), F32&lt;&gt;E32), "_" &amp; TEXT(F32, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C32),"arith_" &amp; INDEX(Operations[],J32,2) &amp; "_g" &amp; TEXT(C32, "00") &amp; "_" &amp; TEXT(D32, "00") &amp; "_o" &amp; TEXT(E32, "00") &amp; IF(AND(ISNUMBER(F32), F32&gt;E32), "_" &amp; TEXT(F32, "00"), ""), "")</f>
         <v>arith_add_g03_00_o08_09</v>
       </c>
       <c r="B32" t="str">
@@ -1746,7 +1756,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>IF(ISNUMBER(C33),"arith_" &amp; INDEX(Operations[],J33,2) &amp; "_g" &amp; TEXT(C33, "00") &amp; "_" &amp; TEXT(D33, "00") &amp; "_o" &amp; TEXT(E33, "00") &amp; IF(AND(ISNUMBER(F33), F33&lt;&gt;E33), "_" &amp; TEXT(F33, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C33),"arith_" &amp; INDEX(Operations[],J33,2) &amp; "_g" &amp; TEXT(C33, "00") &amp; "_" &amp; TEXT(D33, "00") &amp; "_o" &amp; TEXT(E33, "00") &amp; IF(AND(ISNUMBER(F33), F33&gt;E33), "_" &amp; TEXT(F33, "00"), ""), "")</f>
         <v>arith_add_g03_00_o09_10</v>
       </c>
       <c r="B33" t="str">
@@ -1788,7 +1798,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>IF(ISNUMBER(C34),"arith_" &amp; INDEX(Operations[],J34,2) &amp; "_g" &amp; TEXT(C34, "00") &amp; "_" &amp; TEXT(D34, "00") &amp; "_o" &amp; TEXT(E34, "00") &amp; IF(AND(ISNUMBER(F34), F34&lt;&gt;E34), "_" &amp; TEXT(F34, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C34),"arith_" &amp; INDEX(Operations[],J34,2) &amp; "_g" &amp; TEXT(C34, "00") &amp; "_" &amp; TEXT(D34, "00") &amp; "_o" &amp; TEXT(E34, "00") &amp; IF(AND(ISNUMBER(F34), F34&gt;E34), "_" &amp; TEXT(F34, "00"), ""), "")</f>
         <v>arith_add_g03_00_o10</v>
       </c>
       <c r="B34" t="str">
@@ -1830,7 +1840,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>IF(ISNUMBER(C35),"arith_" &amp; INDEX(Operations[],J35,2) &amp; "_g" &amp; TEXT(C35, "00") &amp; "_" &amp; TEXT(D35, "00") &amp; "_o" &amp; TEXT(E35, "00") &amp; IF(AND(ISNUMBER(F35), F35&lt;&gt;E35), "_" &amp; TEXT(F35, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C35),"arith_" &amp; INDEX(Operations[],J35,2) &amp; "_g" &amp; TEXT(C35, "00") &amp; "_" &amp; TEXT(D35, "00") &amp; "_o" &amp; TEXT(E35, "00") &amp; IF(AND(ISNUMBER(F35), F35&gt;E35), "_" &amp; TEXT(F35, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B35" t="str">
@@ -1872,7 +1882,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>IF(ISNUMBER(C36),"arith_" &amp; INDEX(Operations[],J36,2) &amp; "_g" &amp; TEXT(C36, "00") &amp; "_" &amp; TEXT(D36, "00") &amp; "_o" &amp; TEXT(E36, "00") &amp; IF(AND(ISNUMBER(F36), F36&lt;&gt;E36), "_" &amp; TEXT(F36, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C36),"arith_" &amp; INDEX(Operations[],J36,2) &amp; "_g" &amp; TEXT(C36, "00") &amp; "_" &amp; TEXT(D36, "00") &amp; "_o" &amp; TEXT(E36, "00") &amp; IF(AND(ISNUMBER(F36), F36&gt;E36), "_" &amp; TEXT(F36, "00"), ""), "")</f>
         <v>arith_add_g04_00_o01_02</v>
       </c>
       <c r="B36" t="str">
@@ -1914,7 +1924,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>IF(ISNUMBER(C37),"arith_" &amp; INDEX(Operations[],J37,2) &amp; "_g" &amp; TEXT(C37, "00") &amp; "_" &amp; TEXT(D37, "00") &amp; "_o" &amp; TEXT(E37, "00") &amp; IF(AND(ISNUMBER(F37), F37&lt;&gt;E37), "_" &amp; TEXT(F37, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C37),"arith_" &amp; INDEX(Operations[],J37,2) &amp; "_g" &amp; TEXT(C37, "00") &amp; "_" &amp; TEXT(D37, "00") &amp; "_o" &amp; TEXT(E37, "00") &amp; IF(AND(ISNUMBER(F37), F37&gt;E37), "_" &amp; TEXT(F37, "00"), ""), "")</f>
         <v>arith_add_g04_00_o02_03</v>
       </c>
       <c r="B37" t="str">
@@ -1956,7 +1966,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>IF(ISNUMBER(C38),"arith_" &amp; INDEX(Operations[],J38,2) &amp; "_g" &amp; TEXT(C38, "00") &amp; "_" &amp; TEXT(D38, "00") &amp; "_o" &amp; TEXT(E38, "00") &amp; IF(AND(ISNUMBER(F38), F38&lt;&gt;E38), "_" &amp; TEXT(F38, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C38),"arith_" &amp; INDEX(Operations[],J38,2) &amp; "_g" &amp; TEXT(C38, "00") &amp; "_" &amp; TEXT(D38, "00") &amp; "_o" &amp; TEXT(E38, "00") &amp; IF(AND(ISNUMBER(F38), F38&gt;E38), "_" &amp; TEXT(F38, "00"), ""), "")</f>
         <v>arith_add_g04_00_o03_04</v>
       </c>
       <c r="B38" t="str">
@@ -1998,7 +2008,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>IF(ISNUMBER(C39),"arith_" &amp; INDEX(Operations[],J39,2) &amp; "_g" &amp; TEXT(C39, "00") &amp; "_" &amp; TEXT(D39, "00") &amp; "_o" &amp; TEXT(E39, "00") &amp; IF(AND(ISNUMBER(F39), F39&lt;&gt;E39), "_" &amp; TEXT(F39, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C39),"arith_" &amp; INDEX(Operations[],J39,2) &amp; "_g" &amp; TEXT(C39, "00") &amp; "_" &amp; TEXT(D39, "00") &amp; "_o" &amp; TEXT(E39, "00") &amp; IF(AND(ISNUMBER(F39), F39&gt;E39), "_" &amp; TEXT(F39, "00"), ""), "")</f>
         <v>arith_add_g04_00_o04_05</v>
       </c>
       <c r="B39" t="str">
@@ -2040,7 +2050,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>IF(ISNUMBER(C40),"arith_" &amp; INDEX(Operations[],J40,2) &amp; "_g" &amp; TEXT(C40, "00") &amp; "_" &amp; TEXT(D40, "00") &amp; "_o" &amp; TEXT(E40, "00") &amp; IF(AND(ISNUMBER(F40), F40&lt;&gt;E40), "_" &amp; TEXT(F40, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C40),"arith_" &amp; INDEX(Operations[],J40,2) &amp; "_g" &amp; TEXT(C40, "00") &amp; "_" &amp; TEXT(D40, "00") &amp; "_o" &amp; TEXT(E40, "00") &amp; IF(AND(ISNUMBER(F40), F40&gt;E40), "_" &amp; TEXT(F40, "00"), ""), "")</f>
         <v>arith_add_g04_00_o05_06</v>
       </c>
       <c r="B40" t="str">
@@ -2082,7 +2092,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>IF(ISNUMBER(C41),"arith_" &amp; INDEX(Operations[],J41,2) &amp; "_g" &amp; TEXT(C41, "00") &amp; "_" &amp; TEXT(D41, "00") &amp; "_o" &amp; TEXT(E41, "00") &amp; IF(AND(ISNUMBER(F41), F41&lt;&gt;E41), "_" &amp; TEXT(F41, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C41),"arith_" &amp; INDEX(Operations[],J41,2) &amp; "_g" &amp; TEXT(C41, "00") &amp; "_" &amp; TEXT(D41, "00") &amp; "_o" &amp; TEXT(E41, "00") &amp; IF(AND(ISNUMBER(F41), F41&gt;E41), "_" &amp; TEXT(F41, "00"), ""), "")</f>
         <v>arith_add_g04_00_o06_07</v>
       </c>
       <c r="B41" t="str">
@@ -2124,7 +2134,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f>IF(ISNUMBER(C42),"arith_" &amp; INDEX(Operations[],J42,2) &amp; "_g" &amp; TEXT(C42, "00") &amp; "_" &amp; TEXT(D42, "00") &amp; "_o" &amp; TEXT(E42, "00") &amp; IF(AND(ISNUMBER(F42), F42&lt;&gt;E42), "_" &amp; TEXT(F42, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C42),"arith_" &amp; INDEX(Operations[],J42,2) &amp; "_g" &amp; TEXT(C42, "00") &amp; "_" &amp; TEXT(D42, "00") &amp; "_o" &amp; TEXT(E42, "00") &amp; IF(AND(ISNUMBER(F42), F42&gt;E42), "_" &amp; TEXT(F42, "00"), ""), "")</f>
         <v>arith_add_g04_00_o07_08</v>
       </c>
       <c r="B42" t="str">
@@ -2166,7 +2176,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f>IF(ISNUMBER(C43),"arith_" &amp; INDEX(Operations[],J43,2) &amp; "_g" &amp; TEXT(C43, "00") &amp; "_" &amp; TEXT(D43, "00") &amp; "_o" &amp; TEXT(E43, "00") &amp; IF(AND(ISNUMBER(F43), F43&lt;&gt;E43), "_" &amp; TEXT(F43, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C43),"arith_" &amp; INDEX(Operations[],J43,2) &amp; "_g" &amp; TEXT(C43, "00") &amp; "_" &amp; TEXT(D43, "00") &amp; "_o" &amp; TEXT(E43, "00") &amp; IF(AND(ISNUMBER(F43), F43&gt;E43), "_" &amp; TEXT(F43, "00"), ""), "")</f>
         <v>arith_add_g04_00_o08_09</v>
       </c>
       <c r="B43" t="str">
@@ -2208,7 +2218,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f>IF(ISNUMBER(C44),"arith_" &amp; INDEX(Operations[],J44,2) &amp; "_g" &amp; TEXT(C44, "00") &amp; "_" &amp; TEXT(D44, "00") &amp; "_o" &amp; TEXT(E44, "00") &amp; IF(AND(ISNUMBER(F44), F44&lt;&gt;E44), "_" &amp; TEXT(F44, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C44),"arith_" &amp; INDEX(Operations[],J44,2) &amp; "_g" &amp; TEXT(C44, "00") &amp; "_" &amp; TEXT(D44, "00") &amp; "_o" &amp; TEXT(E44, "00") &amp; IF(AND(ISNUMBER(F44), F44&gt;E44), "_" &amp; TEXT(F44, "00"), ""), "")</f>
         <v>arith_add_g04_00_o09_10</v>
       </c>
       <c r="B44" t="str">
@@ -2250,7 +2260,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>IF(ISNUMBER(C45),"arith_" &amp; INDEX(Operations[],J45,2) &amp; "_g" &amp; TEXT(C45, "00") &amp; "_" &amp; TEXT(D45, "00") &amp; "_o" &amp; TEXT(E45, "00") &amp; IF(AND(ISNUMBER(F45), F45&lt;&gt;E45), "_" &amp; TEXT(F45, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C45),"arith_" &amp; INDEX(Operations[],J45,2) &amp; "_g" &amp; TEXT(C45, "00") &amp; "_" &amp; TEXT(D45, "00") &amp; "_o" &amp; TEXT(E45, "00") &amp; IF(AND(ISNUMBER(F45), F45&gt;E45), "_" &amp; TEXT(F45, "00"), ""), "")</f>
         <v>arith_add_g04_00_o10</v>
       </c>
       <c r="B45" t="str">
@@ -2292,7 +2302,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>IF(ISNUMBER(C46),"arith_" &amp; INDEX(Operations[],J46,2) &amp; "_g" &amp; TEXT(C46, "00") &amp; "_" &amp; TEXT(D46, "00") &amp; "_o" &amp; TEXT(E46, "00") &amp; IF(AND(ISNUMBER(F46), F46&lt;&gt;E46), "_" &amp; TEXT(F46, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C46),"arith_" &amp; INDEX(Operations[],J46,2) &amp; "_g" &amp; TEXT(C46, "00") &amp; "_" &amp; TEXT(D46, "00") &amp; "_o" &amp; TEXT(E46, "00") &amp; IF(AND(ISNUMBER(F46), F46&gt;E46), "_" &amp; TEXT(F46, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B46" t="str">
@@ -2334,7 +2344,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f>IF(ISNUMBER(C47),"arith_" &amp; INDEX(Operations[],J47,2) &amp; "_g" &amp; TEXT(C47, "00") &amp; "_" &amp; TEXT(D47, "00") &amp; "_o" &amp; TEXT(E47, "00") &amp; IF(AND(ISNUMBER(F47), F47&lt;&gt;E47), "_" &amp; TEXT(F47, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C47),"arith_" &amp; INDEX(Operations[],J47,2) &amp; "_g" &amp; TEXT(C47, "00") &amp; "_" &amp; TEXT(D47, "00") &amp; "_o" &amp; TEXT(E47, "00") &amp; IF(AND(ISNUMBER(F47), F47&gt;E47), "_" &amp; TEXT(F47, "00"), ""), "")</f>
         <v>arith_add_g05_00_o01_02</v>
       </c>
       <c r="B47" t="str">
@@ -2376,7 +2386,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f>IF(ISNUMBER(C48),"arith_" &amp; INDEX(Operations[],J48,2) &amp; "_g" &amp; TEXT(C48, "00") &amp; "_" &amp; TEXT(D48, "00") &amp; "_o" &amp; TEXT(E48, "00") &amp; IF(AND(ISNUMBER(F48), F48&lt;&gt;E48), "_" &amp; TEXT(F48, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C48),"arith_" &amp; INDEX(Operations[],J48,2) &amp; "_g" &amp; TEXT(C48, "00") &amp; "_" &amp; TEXT(D48, "00") &amp; "_o" &amp; TEXT(E48, "00") &amp; IF(AND(ISNUMBER(F48), F48&gt;E48), "_" &amp; TEXT(F48, "00"), ""), "")</f>
         <v>arith_add_g05_00_o02_03</v>
       </c>
       <c r="B48" t="str">
@@ -2418,7 +2428,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>IF(ISNUMBER(C49),"arith_" &amp; INDEX(Operations[],J49,2) &amp; "_g" &amp; TEXT(C49, "00") &amp; "_" &amp; TEXT(D49, "00") &amp; "_o" &amp; TEXT(E49, "00") &amp; IF(AND(ISNUMBER(F49), F49&lt;&gt;E49), "_" &amp; TEXT(F49, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C49),"arith_" &amp; INDEX(Operations[],J49,2) &amp; "_g" &amp; TEXT(C49, "00") &amp; "_" &amp; TEXT(D49, "00") &amp; "_o" &amp; TEXT(E49, "00") &amp; IF(AND(ISNUMBER(F49), F49&gt;E49), "_" &amp; TEXT(F49, "00"), ""), "")</f>
         <v>arith_add_g05_00_o03_04</v>
       </c>
       <c r="B49" t="str">
@@ -2460,7 +2470,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>IF(ISNUMBER(C50),"arith_" &amp; INDEX(Operations[],J50,2) &amp; "_g" &amp; TEXT(C50, "00") &amp; "_" &amp; TEXT(D50, "00") &amp; "_o" &amp; TEXT(E50, "00") &amp; IF(AND(ISNUMBER(F50), F50&lt;&gt;E50), "_" &amp; TEXT(F50, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C50),"arith_" &amp; INDEX(Operations[],J50,2) &amp; "_g" &amp; TEXT(C50, "00") &amp; "_" &amp; TEXT(D50, "00") &amp; "_o" &amp; TEXT(E50, "00") &amp; IF(AND(ISNUMBER(F50), F50&gt;E50), "_" &amp; TEXT(F50, "00"), ""), "")</f>
         <v>arith_add_g05_00_o04_05</v>
       </c>
       <c r="B50" t="str">
@@ -2502,7 +2512,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f>IF(ISNUMBER(C51),"arith_" &amp; INDEX(Operations[],J51,2) &amp; "_g" &amp; TEXT(C51, "00") &amp; "_" &amp; TEXT(D51, "00") &amp; "_o" &amp; TEXT(E51, "00") &amp; IF(AND(ISNUMBER(F51), F51&lt;&gt;E51), "_" &amp; TEXT(F51, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C51),"arith_" &amp; INDEX(Operations[],J51,2) &amp; "_g" &amp; TEXT(C51, "00") &amp; "_" &amp; TEXT(D51, "00") &amp; "_o" &amp; TEXT(E51, "00") &amp; IF(AND(ISNUMBER(F51), F51&gt;E51), "_" &amp; TEXT(F51, "00"), ""), "")</f>
         <v>arith_add_g05_00_o05_06</v>
       </c>
       <c r="B51" t="str">
@@ -2544,7 +2554,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>IF(ISNUMBER(C52),"arith_" &amp; INDEX(Operations[],J52,2) &amp; "_g" &amp; TEXT(C52, "00") &amp; "_" &amp; TEXT(D52, "00") &amp; "_o" &amp; TEXT(E52, "00") &amp; IF(AND(ISNUMBER(F52), F52&lt;&gt;E52), "_" &amp; TEXT(F52, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C52),"arith_" &amp; INDEX(Operations[],J52,2) &amp; "_g" &amp; TEXT(C52, "00") &amp; "_" &amp; TEXT(D52, "00") &amp; "_o" &amp; TEXT(E52, "00") &amp; IF(AND(ISNUMBER(F52), F52&gt;E52), "_" &amp; TEXT(F52, "00"), ""), "")</f>
         <v>arith_add_g05_00_o06_07</v>
       </c>
       <c r="B52" t="str">
@@ -2586,7 +2596,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f>IF(ISNUMBER(C53),"arith_" &amp; INDEX(Operations[],J53,2) &amp; "_g" &amp; TEXT(C53, "00") &amp; "_" &amp; TEXT(D53, "00") &amp; "_o" &amp; TEXT(E53, "00") &amp; IF(AND(ISNUMBER(F53), F53&lt;&gt;E53), "_" &amp; TEXT(F53, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C53),"arith_" &amp; INDEX(Operations[],J53,2) &amp; "_g" &amp; TEXT(C53, "00") &amp; "_" &amp; TEXT(D53, "00") &amp; "_o" &amp; TEXT(E53, "00") &amp; IF(AND(ISNUMBER(F53), F53&gt;E53), "_" &amp; TEXT(F53, "00"), ""), "")</f>
         <v>arith_add_g05_00_o07_08</v>
       </c>
       <c r="B53" t="str">
@@ -2628,7 +2638,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f>IF(ISNUMBER(C54),"arith_" &amp; INDEX(Operations[],J54,2) &amp; "_g" &amp; TEXT(C54, "00") &amp; "_" &amp; TEXT(D54, "00") &amp; "_o" &amp; TEXT(E54, "00") &amp; IF(AND(ISNUMBER(F54), F54&lt;&gt;E54), "_" &amp; TEXT(F54, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C54),"arith_" &amp; INDEX(Operations[],J54,2) &amp; "_g" &amp; TEXT(C54, "00") &amp; "_" &amp; TEXT(D54, "00") &amp; "_o" &amp; TEXT(E54, "00") &amp; IF(AND(ISNUMBER(F54), F54&gt;E54), "_" &amp; TEXT(F54, "00"), ""), "")</f>
         <v>arith_add_g05_00_o08_09</v>
       </c>
       <c r="B54" t="str">
@@ -2670,7 +2680,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f>IF(ISNUMBER(C55),"arith_" &amp; INDEX(Operations[],J55,2) &amp; "_g" &amp; TEXT(C55, "00") &amp; "_" &amp; TEXT(D55, "00") &amp; "_o" &amp; TEXT(E55, "00") &amp; IF(AND(ISNUMBER(F55), F55&lt;&gt;E55), "_" &amp; TEXT(F55, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C55),"arith_" &amp; INDEX(Operations[],J55,2) &amp; "_g" &amp; TEXT(C55, "00") &amp; "_" &amp; TEXT(D55, "00") &amp; "_o" &amp; TEXT(E55, "00") &amp; IF(AND(ISNUMBER(F55), F55&gt;E55), "_" &amp; TEXT(F55, "00"), ""), "")</f>
         <v>arith_add_g05_00_o09_10</v>
       </c>
       <c r="B55" t="str">
@@ -2712,7 +2722,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>IF(ISNUMBER(C56),"arith_" &amp; INDEX(Operations[],J56,2) &amp; "_g" &amp; TEXT(C56, "00") &amp; "_" &amp; TEXT(D56, "00") &amp; "_o" &amp; TEXT(E56, "00") &amp; IF(AND(ISNUMBER(F56), F56&lt;&gt;E56), "_" &amp; TEXT(F56, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C56),"arith_" &amp; INDEX(Operations[],J56,2) &amp; "_g" &amp; TEXT(C56, "00") &amp; "_" &amp; TEXT(D56, "00") &amp; "_o" &amp; TEXT(E56, "00") &amp; IF(AND(ISNUMBER(F56), F56&gt;E56), "_" &amp; TEXT(F56, "00"), ""), "")</f>
         <v>arith_add_g05_00_o10</v>
       </c>
       <c r="B56" t="str">
@@ -2754,7 +2764,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f>IF(ISNUMBER(C57),"arith_" &amp; INDEX(Operations[],J57,2) &amp; "_g" &amp; TEXT(C57, "00") &amp; "_" &amp; TEXT(D57, "00") &amp; "_o" &amp; TEXT(E57, "00") &amp; IF(AND(ISNUMBER(F57), F57&lt;&gt;E57), "_" &amp; TEXT(F57, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C57),"arith_" &amp; INDEX(Operations[],J57,2) &amp; "_g" &amp; TEXT(C57, "00") &amp; "_" &amp; TEXT(D57, "00") &amp; "_o" &amp; TEXT(E57, "00") &amp; IF(AND(ISNUMBER(F57), F57&gt;E57), "_" &amp; TEXT(F57, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B57" t="str">
@@ -2796,7 +2806,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f>IF(ISNUMBER(C58),"arith_" &amp; INDEX(Operations[],J58,2) &amp; "_g" &amp; TEXT(C58, "00") &amp; "_" &amp; TEXT(D58, "00") &amp; "_o" &amp; TEXT(E58, "00") &amp; IF(AND(ISNUMBER(F58), F58&lt;&gt;E58), "_" &amp; TEXT(F58, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C58),"arith_" &amp; INDEX(Operations[],J58,2) &amp; "_g" &amp; TEXT(C58, "00") &amp; "_" &amp; TEXT(D58, "00") &amp; "_o" &amp; TEXT(E58, "00") &amp; IF(AND(ISNUMBER(F58), F58&gt;E58), "_" &amp; TEXT(F58, "00"), ""), "")</f>
         <v>arith_add_g06_00_o01_02</v>
       </c>
       <c r="B58" t="str">
@@ -2838,7 +2848,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f>IF(ISNUMBER(C59),"arith_" &amp; INDEX(Operations[],J59,2) &amp; "_g" &amp; TEXT(C59, "00") &amp; "_" &amp; TEXT(D59, "00") &amp; "_o" &amp; TEXT(E59, "00") &amp; IF(AND(ISNUMBER(F59), F59&lt;&gt;E59), "_" &amp; TEXT(F59, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C59),"arith_" &amp; INDEX(Operations[],J59,2) &amp; "_g" &amp; TEXT(C59, "00") &amp; "_" &amp; TEXT(D59, "00") &amp; "_o" &amp; TEXT(E59, "00") &amp; IF(AND(ISNUMBER(F59), F59&gt;E59), "_" &amp; TEXT(F59, "00"), ""), "")</f>
         <v>arith_add_g06_00_o02_03</v>
       </c>
       <c r="B59" t="str">
@@ -2880,7 +2890,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>IF(ISNUMBER(C60),"arith_" &amp; INDEX(Operations[],J60,2) &amp; "_g" &amp; TEXT(C60, "00") &amp; "_" &amp; TEXT(D60, "00") &amp; "_o" &amp; TEXT(E60, "00") &amp; IF(AND(ISNUMBER(F60), F60&lt;&gt;E60), "_" &amp; TEXT(F60, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C60),"arith_" &amp; INDEX(Operations[],J60,2) &amp; "_g" &amp; TEXT(C60, "00") &amp; "_" &amp; TEXT(D60, "00") &amp; "_o" &amp; TEXT(E60, "00") &amp; IF(AND(ISNUMBER(F60), F60&gt;E60), "_" &amp; TEXT(F60, "00"), ""), "")</f>
         <v>arith_add_g06_00_o03_04</v>
       </c>
       <c r="B60" t="str">
@@ -2922,7 +2932,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f>IF(ISNUMBER(C61),"arith_" &amp; INDEX(Operations[],J61,2) &amp; "_g" &amp; TEXT(C61, "00") &amp; "_" &amp; TEXT(D61, "00") &amp; "_o" &amp; TEXT(E61, "00") &amp; IF(AND(ISNUMBER(F61), F61&lt;&gt;E61), "_" &amp; TEXT(F61, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C61),"arith_" &amp; INDEX(Operations[],J61,2) &amp; "_g" &amp; TEXT(C61, "00") &amp; "_" &amp; TEXT(D61, "00") &amp; "_o" &amp; TEXT(E61, "00") &amp; IF(AND(ISNUMBER(F61), F61&gt;E61), "_" &amp; TEXT(F61, "00"), ""), "")</f>
         <v>arith_add_g06_00_o04_05</v>
       </c>
       <c r="B61" t="str">
@@ -2964,7 +2974,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f>IF(ISNUMBER(C62),"arith_" &amp; INDEX(Operations[],J62,2) &amp; "_g" &amp; TEXT(C62, "00") &amp; "_" &amp; TEXT(D62, "00") &amp; "_o" &amp; TEXT(E62, "00") &amp; IF(AND(ISNUMBER(F62), F62&lt;&gt;E62), "_" &amp; TEXT(F62, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C62),"arith_" &amp; INDEX(Operations[],J62,2) &amp; "_g" &amp; TEXT(C62, "00") &amp; "_" &amp; TEXT(D62, "00") &amp; "_o" &amp; TEXT(E62, "00") &amp; IF(AND(ISNUMBER(F62), F62&gt;E62), "_" &amp; TEXT(F62, "00"), ""), "")</f>
         <v>arith_add_g06_00_o05_06</v>
       </c>
       <c r="B62" t="str">
@@ -3006,7 +3016,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f>IF(ISNUMBER(C63),"arith_" &amp; INDEX(Operations[],J63,2) &amp; "_g" &amp; TEXT(C63, "00") &amp; "_" &amp; TEXT(D63, "00") &amp; "_o" &amp; TEXT(E63, "00") &amp; IF(AND(ISNUMBER(F63), F63&lt;&gt;E63), "_" &amp; TEXT(F63, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C63),"arith_" &amp; INDEX(Operations[],J63,2) &amp; "_g" &amp; TEXT(C63, "00") &amp; "_" &amp; TEXT(D63, "00") &amp; "_o" &amp; TEXT(E63, "00") &amp; IF(AND(ISNUMBER(F63), F63&gt;E63), "_" &amp; TEXT(F63, "00"), ""), "")</f>
         <v>arith_add_g06_00_o06_07</v>
       </c>
       <c r="B63" t="str">
@@ -3048,7 +3058,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f>IF(ISNUMBER(C64),"arith_" &amp; INDEX(Operations[],J64,2) &amp; "_g" &amp; TEXT(C64, "00") &amp; "_" &amp; TEXT(D64, "00") &amp; "_o" &amp; TEXT(E64, "00") &amp; IF(AND(ISNUMBER(F64), F64&lt;&gt;E64), "_" &amp; TEXT(F64, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C64),"arith_" &amp; INDEX(Operations[],J64,2) &amp; "_g" &amp; TEXT(C64, "00") &amp; "_" &amp; TEXT(D64, "00") &amp; "_o" &amp; TEXT(E64, "00") &amp; IF(AND(ISNUMBER(F64), F64&gt;E64), "_" &amp; TEXT(F64, "00"), ""), "")</f>
         <v>arith_add_g06_00_o07_08</v>
       </c>
       <c r="B64" t="str">
@@ -3090,7 +3100,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f>IF(ISNUMBER(C65),"arith_" &amp; INDEX(Operations[],J65,2) &amp; "_g" &amp; TEXT(C65, "00") &amp; "_" &amp; TEXT(D65, "00") &amp; "_o" &amp; TEXT(E65, "00") &amp; IF(AND(ISNUMBER(F65), F65&lt;&gt;E65), "_" &amp; TEXT(F65, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C65),"arith_" &amp; INDEX(Operations[],J65,2) &amp; "_g" &amp; TEXT(C65, "00") &amp; "_" &amp; TEXT(D65, "00") &amp; "_o" &amp; TEXT(E65, "00") &amp; IF(AND(ISNUMBER(F65), F65&gt;E65), "_" &amp; TEXT(F65, "00"), ""), "")</f>
         <v>arith_add_g06_00_o08_09</v>
       </c>
       <c r="B65" t="str">
@@ -3132,7 +3142,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f>IF(ISNUMBER(C66),"arith_" &amp; INDEX(Operations[],J66,2) &amp; "_g" &amp; TEXT(C66, "00") &amp; "_" &amp; TEXT(D66, "00") &amp; "_o" &amp; TEXT(E66, "00") &amp; IF(AND(ISNUMBER(F66), F66&lt;&gt;E66), "_" &amp; TEXT(F66, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C66),"arith_" &amp; INDEX(Operations[],J66,2) &amp; "_g" &amp; TEXT(C66, "00") &amp; "_" &amp; TEXT(D66, "00") &amp; "_o" &amp; TEXT(E66, "00") &amp; IF(AND(ISNUMBER(F66), F66&gt;E66), "_" &amp; TEXT(F66, "00"), ""), "")</f>
         <v>arith_add_g06_00_o09_10</v>
       </c>
       <c r="B66" t="str">
@@ -3174,7 +3184,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f>IF(ISNUMBER(C67),"arith_" &amp; INDEX(Operations[],J67,2) &amp; "_g" &amp; TEXT(C67, "00") &amp; "_" &amp; TEXT(D67, "00") &amp; "_o" &amp; TEXT(E67, "00") &amp; IF(AND(ISNUMBER(F67), F67&lt;&gt;E67), "_" &amp; TEXT(F67, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C67),"arith_" &amp; INDEX(Operations[],J67,2) &amp; "_g" &amp; TEXT(C67, "00") &amp; "_" &amp; TEXT(D67, "00") &amp; "_o" &amp; TEXT(E67, "00") &amp; IF(AND(ISNUMBER(F67), F67&gt;E67), "_" &amp; TEXT(F67, "00"), ""), "")</f>
         <v>arith_add_g06_00_o10</v>
       </c>
       <c r="B67" t="str">
@@ -3216,7 +3226,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f>IF(ISNUMBER(C68),"arith_" &amp; INDEX(Operations[],J68,2) &amp; "_g" &amp; TEXT(C68, "00") &amp; "_" &amp; TEXT(D68, "00") &amp; "_o" &amp; TEXT(E68, "00") &amp; IF(AND(ISNUMBER(F68), F68&lt;&gt;E68), "_" &amp; TEXT(F68, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C68),"arith_" &amp; INDEX(Operations[],J68,2) &amp; "_g" &amp; TEXT(C68, "00") &amp; "_" &amp; TEXT(D68, "00") &amp; "_o" &amp; TEXT(E68, "00") &amp; IF(AND(ISNUMBER(F68), F68&gt;E68), "_" &amp; TEXT(F68, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B68" t="str">
@@ -3258,7 +3268,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f>IF(ISNUMBER(C69),"arith_" &amp; INDEX(Operations[],J69,2) &amp; "_g" &amp; TEXT(C69, "00") &amp; "_" &amp; TEXT(D69, "00") &amp; "_o" &amp; TEXT(E69, "00") &amp; IF(AND(ISNUMBER(F69), F69&lt;&gt;E69), "_" &amp; TEXT(F69, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C69),"arith_" &amp; INDEX(Operations[],J69,2) &amp; "_g" &amp; TEXT(C69, "00") &amp; "_" &amp; TEXT(D69, "00") &amp; "_o" &amp; TEXT(E69, "00") &amp; IF(AND(ISNUMBER(F69), F69&gt;E69), "_" &amp; TEXT(F69, "00"), ""), "")</f>
         <v>arith_add_g07_00_o01_02</v>
       </c>
       <c r="B69" t="str">
@@ -3300,7 +3310,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f>IF(ISNUMBER(C70),"arith_" &amp; INDEX(Operations[],J70,2) &amp; "_g" &amp; TEXT(C70, "00") &amp; "_" &amp; TEXT(D70, "00") &amp; "_o" &amp; TEXT(E70, "00") &amp; IF(AND(ISNUMBER(F70), F70&lt;&gt;E70), "_" &amp; TEXT(F70, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C70),"arith_" &amp; INDEX(Operations[],J70,2) &amp; "_g" &amp; TEXT(C70, "00") &amp; "_" &amp; TEXT(D70, "00") &amp; "_o" &amp; TEXT(E70, "00") &amp; IF(AND(ISNUMBER(F70), F70&gt;E70), "_" &amp; TEXT(F70, "00"), ""), "")</f>
         <v>arith_add_g07_00_o02_03</v>
       </c>
       <c r="B70" t="str">
@@ -3342,7 +3352,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f>IF(ISNUMBER(C71),"arith_" &amp; INDEX(Operations[],J71,2) &amp; "_g" &amp; TEXT(C71, "00") &amp; "_" &amp; TEXT(D71, "00") &amp; "_o" &amp; TEXT(E71, "00") &amp; IF(AND(ISNUMBER(F71), F71&lt;&gt;E71), "_" &amp; TEXT(F71, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C71),"arith_" &amp; INDEX(Operations[],J71,2) &amp; "_g" &amp; TEXT(C71, "00") &amp; "_" &amp; TEXT(D71, "00") &amp; "_o" &amp; TEXT(E71, "00") &amp; IF(AND(ISNUMBER(F71), F71&gt;E71), "_" &amp; TEXT(F71, "00"), ""), "")</f>
         <v>arith_add_g07_00_o03_04</v>
       </c>
       <c r="B71" t="str">
@@ -3384,7 +3394,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f>IF(ISNUMBER(C72),"arith_" &amp; INDEX(Operations[],J72,2) &amp; "_g" &amp; TEXT(C72, "00") &amp; "_" &amp; TEXT(D72, "00") &amp; "_o" &amp; TEXT(E72, "00") &amp; IF(AND(ISNUMBER(F72), F72&lt;&gt;E72), "_" &amp; TEXT(F72, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C72),"arith_" &amp; INDEX(Operations[],J72,2) &amp; "_g" &amp; TEXT(C72, "00") &amp; "_" &amp; TEXT(D72, "00") &amp; "_o" &amp; TEXT(E72, "00") &amp; IF(AND(ISNUMBER(F72), F72&gt;E72), "_" &amp; TEXT(F72, "00"), ""), "")</f>
         <v>arith_add_g07_00_o04_05</v>
       </c>
       <c r="B72" t="str">
@@ -3426,7 +3436,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f>IF(ISNUMBER(C73),"arith_" &amp; INDEX(Operations[],J73,2) &amp; "_g" &amp; TEXT(C73, "00") &amp; "_" &amp; TEXT(D73, "00") &amp; "_o" &amp; TEXT(E73, "00") &amp; IF(AND(ISNUMBER(F73), F73&lt;&gt;E73), "_" &amp; TEXT(F73, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C73),"arith_" &amp; INDEX(Operations[],J73,2) &amp; "_g" &amp; TEXT(C73, "00") &amp; "_" &amp; TEXT(D73, "00") &amp; "_o" &amp; TEXT(E73, "00") &amp; IF(AND(ISNUMBER(F73), F73&gt;E73), "_" &amp; TEXT(F73, "00"), ""), "")</f>
         <v>arith_add_g07_00_o05_06</v>
       </c>
       <c r="B73" t="str">
@@ -3468,7 +3478,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f>IF(ISNUMBER(C74),"arith_" &amp; INDEX(Operations[],J74,2) &amp; "_g" &amp; TEXT(C74, "00") &amp; "_" &amp; TEXT(D74, "00") &amp; "_o" &amp; TEXT(E74, "00") &amp; IF(AND(ISNUMBER(F74), F74&lt;&gt;E74), "_" &amp; TEXT(F74, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C74),"arith_" &amp; INDEX(Operations[],J74,2) &amp; "_g" &amp; TEXT(C74, "00") &amp; "_" &amp; TEXT(D74, "00") &amp; "_o" &amp; TEXT(E74, "00") &amp; IF(AND(ISNUMBER(F74), F74&gt;E74), "_" &amp; TEXT(F74, "00"), ""), "")</f>
         <v>arith_add_g07_00_o06_07</v>
       </c>
       <c r="B74" t="str">
@@ -3510,7 +3520,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f>IF(ISNUMBER(C75),"arith_" &amp; INDEX(Operations[],J75,2) &amp; "_g" &amp; TEXT(C75, "00") &amp; "_" &amp; TEXT(D75, "00") &amp; "_o" &amp; TEXT(E75, "00") &amp; IF(AND(ISNUMBER(F75), F75&lt;&gt;E75), "_" &amp; TEXT(F75, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C75),"arith_" &amp; INDEX(Operations[],J75,2) &amp; "_g" &amp; TEXT(C75, "00") &amp; "_" &amp; TEXT(D75, "00") &amp; "_o" &amp; TEXT(E75, "00") &amp; IF(AND(ISNUMBER(F75), F75&gt;E75), "_" &amp; TEXT(F75, "00"), ""), "")</f>
         <v>arith_add_g07_00_o07_08</v>
       </c>
       <c r="B75" t="str">
@@ -3552,7 +3562,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
-        <f>IF(ISNUMBER(C76),"arith_" &amp; INDEX(Operations[],J76,2) &amp; "_g" &amp; TEXT(C76, "00") &amp; "_" &amp; TEXT(D76, "00") &amp; "_o" &amp; TEXT(E76, "00") &amp; IF(AND(ISNUMBER(F76), F76&lt;&gt;E76), "_" &amp; TEXT(F76, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C76),"arith_" &amp; INDEX(Operations[],J76,2) &amp; "_g" &amp; TEXT(C76, "00") &amp; "_" &amp; TEXT(D76, "00") &amp; "_o" &amp; TEXT(E76, "00") &amp; IF(AND(ISNUMBER(F76), F76&gt;E76), "_" &amp; TEXT(F76, "00"), ""), "")</f>
         <v>arith_add_g07_00_o08_09</v>
       </c>
       <c r="B76" t="str">
@@ -3594,7 +3604,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
-        <f>IF(ISNUMBER(C77),"arith_" &amp; INDEX(Operations[],J77,2) &amp; "_g" &amp; TEXT(C77, "00") &amp; "_" &amp; TEXT(D77, "00") &amp; "_o" &amp; TEXT(E77, "00") &amp; IF(AND(ISNUMBER(F77), F77&lt;&gt;E77), "_" &amp; TEXT(F77, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C77),"arith_" &amp; INDEX(Operations[],J77,2) &amp; "_g" &amp; TEXT(C77, "00") &amp; "_" &amp; TEXT(D77, "00") &amp; "_o" &amp; TEXT(E77, "00") &amp; IF(AND(ISNUMBER(F77), F77&gt;E77), "_" &amp; TEXT(F77, "00"), ""), "")</f>
         <v>arith_add_g07_00_o09_10</v>
       </c>
       <c r="B77" t="str">
@@ -3636,7 +3646,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="str">
-        <f>IF(ISNUMBER(C78),"arith_" &amp; INDEX(Operations[],J78,2) &amp; "_g" &amp; TEXT(C78, "00") &amp; "_" &amp; TEXT(D78, "00") &amp; "_o" &amp; TEXT(E78, "00") &amp; IF(AND(ISNUMBER(F78), F78&lt;&gt;E78), "_" &amp; TEXT(F78, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C78),"arith_" &amp; INDEX(Operations[],J78,2) &amp; "_g" &amp; TEXT(C78, "00") &amp; "_" &amp; TEXT(D78, "00") &amp; "_o" &amp; TEXT(E78, "00") &amp; IF(AND(ISNUMBER(F78), F78&gt;E78), "_" &amp; TEXT(F78, "00"), ""), "")</f>
         <v>arith_add_g07_00_o10</v>
       </c>
       <c r="B78" t="str">
@@ -3678,7 +3688,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="str">
-        <f>IF(ISNUMBER(C79),"arith_" &amp; INDEX(Operations[],J79,2) &amp; "_g" &amp; TEXT(C79, "00") &amp; "_" &amp; TEXT(D79, "00") &amp; "_o" &amp; TEXT(E79, "00") &amp; IF(AND(ISNUMBER(F79), F79&lt;&gt;E79), "_" &amp; TEXT(F79, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C79),"arith_" &amp; INDEX(Operations[],J79,2) &amp; "_g" &amp; TEXT(C79, "00") &amp; "_" &amp; TEXT(D79, "00") &amp; "_o" &amp; TEXT(E79, "00") &amp; IF(AND(ISNUMBER(F79), F79&gt;E79), "_" &amp; TEXT(F79, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B79" t="str">
@@ -3720,7 +3730,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="str">
-        <f>IF(ISNUMBER(C80),"arith_" &amp; INDEX(Operations[],J80,2) &amp; "_g" &amp; TEXT(C80, "00") &amp; "_" &amp; TEXT(D80, "00") &amp; "_o" &amp; TEXT(E80, "00") &amp; IF(AND(ISNUMBER(F80), F80&lt;&gt;E80), "_" &amp; TEXT(F80, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C80),"arith_" &amp; INDEX(Operations[],J80,2) &amp; "_g" &amp; TEXT(C80, "00") &amp; "_" &amp; TEXT(D80, "00") &amp; "_o" &amp; TEXT(E80, "00") &amp; IF(AND(ISNUMBER(F80), F80&gt;E80), "_" &amp; TEXT(F80, "00"), ""), "")</f>
         <v>arith_add_g08_00_o01_02</v>
       </c>
       <c r="B80" t="str">
@@ -3762,7 +3772,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="str">
-        <f>IF(ISNUMBER(C81),"arith_" &amp; INDEX(Operations[],J81,2) &amp; "_g" &amp; TEXT(C81, "00") &amp; "_" &amp; TEXT(D81, "00") &amp; "_o" &amp; TEXT(E81, "00") &amp; IF(AND(ISNUMBER(F81), F81&lt;&gt;E81), "_" &amp; TEXT(F81, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C81),"arith_" &amp; INDEX(Operations[],J81,2) &amp; "_g" &amp; TEXT(C81, "00") &amp; "_" &amp; TEXT(D81, "00") &amp; "_o" &amp; TEXT(E81, "00") &amp; IF(AND(ISNUMBER(F81), F81&gt;E81), "_" &amp; TEXT(F81, "00"), ""), "")</f>
         <v>arith_add_g08_00_o02_03</v>
       </c>
       <c r="B81" t="str">
@@ -3804,7 +3814,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="str">
-        <f>IF(ISNUMBER(C82),"arith_" &amp; INDEX(Operations[],J82,2) &amp; "_g" &amp; TEXT(C82, "00") &amp; "_" &amp; TEXT(D82, "00") &amp; "_o" &amp; TEXT(E82, "00") &amp; IF(AND(ISNUMBER(F82), F82&lt;&gt;E82), "_" &amp; TEXT(F82, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C82),"arith_" &amp; INDEX(Operations[],J82,2) &amp; "_g" &amp; TEXT(C82, "00") &amp; "_" &amp; TEXT(D82, "00") &amp; "_o" &amp; TEXT(E82, "00") &amp; IF(AND(ISNUMBER(F82), F82&gt;E82), "_" &amp; TEXT(F82, "00"), ""), "")</f>
         <v>arith_add_g08_00_o03_04</v>
       </c>
       <c r="B82" t="str">
@@ -3846,7 +3856,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
-        <f>IF(ISNUMBER(C83),"arith_" &amp; INDEX(Operations[],J83,2) &amp; "_g" &amp; TEXT(C83, "00") &amp; "_" &amp; TEXT(D83, "00") &amp; "_o" &amp; TEXT(E83, "00") &amp; IF(AND(ISNUMBER(F83), F83&lt;&gt;E83), "_" &amp; TEXT(F83, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C83),"arith_" &amp; INDEX(Operations[],J83,2) &amp; "_g" &amp; TEXT(C83, "00") &amp; "_" &amp; TEXT(D83, "00") &amp; "_o" &amp; TEXT(E83, "00") &amp; IF(AND(ISNUMBER(F83), F83&gt;E83), "_" &amp; TEXT(F83, "00"), ""), "")</f>
         <v>arith_add_g08_00_o04_05</v>
       </c>
       <c r="B83" t="str">
@@ -3888,7 +3898,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="str">
-        <f>IF(ISNUMBER(C84),"arith_" &amp; INDEX(Operations[],J84,2) &amp; "_g" &amp; TEXT(C84, "00") &amp; "_" &amp; TEXT(D84, "00") &amp; "_o" &amp; TEXT(E84, "00") &amp; IF(AND(ISNUMBER(F84), F84&lt;&gt;E84), "_" &amp; TEXT(F84, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C84),"arith_" &amp; INDEX(Operations[],J84,2) &amp; "_g" &amp; TEXT(C84, "00") &amp; "_" &amp; TEXT(D84, "00") &amp; "_o" &amp; TEXT(E84, "00") &amp; IF(AND(ISNUMBER(F84), F84&gt;E84), "_" &amp; TEXT(F84, "00"), ""), "")</f>
         <v>arith_add_g08_00_o05_06</v>
       </c>
       <c r="B84" t="str">
@@ -3930,7 +3940,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="str">
-        <f>IF(ISNUMBER(C85),"arith_" &amp; INDEX(Operations[],J85,2) &amp; "_g" &amp; TEXT(C85, "00") &amp; "_" &amp; TEXT(D85, "00") &amp; "_o" &amp; TEXT(E85, "00") &amp; IF(AND(ISNUMBER(F85), F85&lt;&gt;E85), "_" &amp; TEXT(F85, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C85),"arith_" &amp; INDEX(Operations[],J85,2) &amp; "_g" &amp; TEXT(C85, "00") &amp; "_" &amp; TEXT(D85, "00") &amp; "_o" &amp; TEXT(E85, "00") &amp; IF(AND(ISNUMBER(F85), F85&gt;E85), "_" &amp; TEXT(F85, "00"), ""), "")</f>
         <v>arith_add_g08_00_o06_07</v>
       </c>
       <c r="B85" t="str">
@@ -3972,7 +3982,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="str">
-        <f>IF(ISNUMBER(C86),"arith_" &amp; INDEX(Operations[],J86,2) &amp; "_g" &amp; TEXT(C86, "00") &amp; "_" &amp; TEXT(D86, "00") &amp; "_o" &amp; TEXT(E86, "00") &amp; IF(AND(ISNUMBER(F86), F86&lt;&gt;E86), "_" &amp; TEXT(F86, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C86),"arith_" &amp; INDEX(Operations[],J86,2) &amp; "_g" &amp; TEXT(C86, "00") &amp; "_" &amp; TEXT(D86, "00") &amp; "_o" &amp; TEXT(E86, "00") &amp; IF(AND(ISNUMBER(F86), F86&gt;E86), "_" &amp; TEXT(F86, "00"), ""), "")</f>
         <v>arith_add_g08_00_o07_08</v>
       </c>
       <c r="B86" t="str">
@@ -4014,7 +4024,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="str">
-        <f>IF(ISNUMBER(C87),"arith_" &amp; INDEX(Operations[],J87,2) &amp; "_g" &amp; TEXT(C87, "00") &amp; "_" &amp; TEXT(D87, "00") &amp; "_o" &amp; TEXT(E87, "00") &amp; IF(AND(ISNUMBER(F87), F87&lt;&gt;E87), "_" &amp; TEXT(F87, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C87),"arith_" &amp; INDEX(Operations[],J87,2) &amp; "_g" &amp; TEXT(C87, "00") &amp; "_" &amp; TEXT(D87, "00") &amp; "_o" &amp; TEXT(E87, "00") &amp; IF(AND(ISNUMBER(F87), F87&gt;E87), "_" &amp; TEXT(F87, "00"), ""), "")</f>
         <v>arith_add_g08_00_o08_09</v>
       </c>
       <c r="B87" t="str">
@@ -4056,7 +4066,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="str">
-        <f>IF(ISNUMBER(C88),"arith_" &amp; INDEX(Operations[],J88,2) &amp; "_g" &amp; TEXT(C88, "00") &amp; "_" &amp; TEXT(D88, "00") &amp; "_o" &amp; TEXT(E88, "00") &amp; IF(AND(ISNUMBER(F88), F88&lt;&gt;E88), "_" &amp; TEXT(F88, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C88),"arith_" &amp; INDEX(Operations[],J88,2) &amp; "_g" &amp; TEXT(C88, "00") &amp; "_" &amp; TEXT(D88, "00") &amp; "_o" &amp; TEXT(E88, "00") &amp; IF(AND(ISNUMBER(F88), F88&gt;E88), "_" &amp; TEXT(F88, "00"), ""), "")</f>
         <v>arith_add_g08_00_o09_10</v>
       </c>
       <c r="B88" t="str">
@@ -4098,7 +4108,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="str">
-        <f>IF(ISNUMBER(C89),"arith_" &amp; INDEX(Operations[],J89,2) &amp; "_g" &amp; TEXT(C89, "00") &amp; "_" &amp; TEXT(D89, "00") &amp; "_o" &amp; TEXT(E89, "00") &amp; IF(AND(ISNUMBER(F89), F89&lt;&gt;E89), "_" &amp; TEXT(F89, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C89),"arith_" &amp; INDEX(Operations[],J89,2) &amp; "_g" &amp; TEXT(C89, "00") &amp; "_" &amp; TEXT(D89, "00") &amp; "_o" &amp; TEXT(E89, "00") &amp; IF(AND(ISNUMBER(F89), F89&gt;E89), "_" &amp; TEXT(F89, "00"), ""), "")</f>
         <v>arith_add_g08_00_o10</v>
       </c>
       <c r="B89" t="str">
@@ -4140,7 +4150,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="str">
-        <f>IF(ISNUMBER(C90),"arith_" &amp; INDEX(Operations[],J90,2) &amp; "_g" &amp; TEXT(C90, "00") &amp; "_" &amp; TEXT(D90, "00") &amp; "_o" &amp; TEXT(E90, "00") &amp; IF(AND(ISNUMBER(F90), F90&lt;&gt;E90), "_" &amp; TEXT(F90, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C90),"arith_" &amp; INDEX(Operations[],J90,2) &amp; "_g" &amp; TEXT(C90, "00") &amp; "_" &amp; TEXT(D90, "00") &amp; "_o" &amp; TEXT(E90, "00") &amp; IF(AND(ISNUMBER(F90), F90&gt;E90), "_" &amp; TEXT(F90, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B90" t="str">
@@ -4182,7 +4192,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="str">
-        <f>IF(ISNUMBER(C91),"arith_" &amp; INDEX(Operations[],J91,2) &amp; "_g" &amp; TEXT(C91, "00") &amp; "_" &amp; TEXT(D91, "00") &amp; "_o" &amp; TEXT(E91, "00") &amp; IF(AND(ISNUMBER(F91), F91&lt;&gt;E91), "_" &amp; TEXT(F91, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C91),"arith_" &amp; INDEX(Operations[],J91,2) &amp; "_g" &amp; TEXT(C91, "00") &amp; "_" &amp; TEXT(D91, "00") &amp; "_o" &amp; TEXT(E91, "00") &amp; IF(AND(ISNUMBER(F91), F91&gt;E91), "_" &amp; TEXT(F91, "00"), ""), "")</f>
         <v>arith_add_g09_00_o01_02</v>
       </c>
       <c r="B91" t="str">
@@ -4224,7 +4234,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="str">
-        <f>IF(ISNUMBER(C92),"arith_" &amp; INDEX(Operations[],J92,2) &amp; "_g" &amp; TEXT(C92, "00") &amp; "_" &amp; TEXT(D92, "00") &amp; "_o" &amp; TEXT(E92, "00") &amp; IF(AND(ISNUMBER(F92), F92&lt;&gt;E92), "_" &amp; TEXT(F92, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C92),"arith_" &amp; INDEX(Operations[],J92,2) &amp; "_g" &amp; TEXT(C92, "00") &amp; "_" &amp; TEXT(D92, "00") &amp; "_o" &amp; TEXT(E92, "00") &amp; IF(AND(ISNUMBER(F92), F92&gt;E92), "_" &amp; TEXT(F92, "00"), ""), "")</f>
         <v>arith_add_g09_00_o02_03</v>
       </c>
       <c r="B92" t="str">
@@ -4266,7 +4276,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="str">
-        <f>IF(ISNUMBER(C93),"arith_" &amp; INDEX(Operations[],J93,2) &amp; "_g" &amp; TEXT(C93, "00") &amp; "_" &amp; TEXT(D93, "00") &amp; "_o" &amp; TEXT(E93, "00") &amp; IF(AND(ISNUMBER(F93), F93&lt;&gt;E93), "_" &amp; TEXT(F93, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C93),"arith_" &amp; INDEX(Operations[],J93,2) &amp; "_g" &amp; TEXT(C93, "00") &amp; "_" &amp; TEXT(D93, "00") &amp; "_o" &amp; TEXT(E93, "00") &amp; IF(AND(ISNUMBER(F93), F93&gt;E93), "_" &amp; TEXT(F93, "00"), ""), "")</f>
         <v>arith_add_g09_00_o03_04</v>
       </c>
       <c r="B93" t="str">
@@ -4308,7 +4318,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="str">
-        <f>IF(ISNUMBER(C94),"arith_" &amp; INDEX(Operations[],J94,2) &amp; "_g" &amp; TEXT(C94, "00") &amp; "_" &amp; TEXT(D94, "00") &amp; "_o" &amp; TEXT(E94, "00") &amp; IF(AND(ISNUMBER(F94), F94&lt;&gt;E94), "_" &amp; TEXT(F94, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C94),"arith_" &amp; INDEX(Operations[],J94,2) &amp; "_g" &amp; TEXT(C94, "00") &amp; "_" &amp; TEXT(D94, "00") &amp; "_o" &amp; TEXT(E94, "00") &amp; IF(AND(ISNUMBER(F94), F94&gt;E94), "_" &amp; TEXT(F94, "00"), ""), "")</f>
         <v>arith_add_g09_00_o04_05</v>
       </c>
       <c r="B94" t="str">
@@ -4350,7 +4360,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="str">
-        <f>IF(ISNUMBER(C95),"arith_" &amp; INDEX(Operations[],J95,2) &amp; "_g" &amp; TEXT(C95, "00") &amp; "_" &amp; TEXT(D95, "00") &amp; "_o" &amp; TEXT(E95, "00") &amp; IF(AND(ISNUMBER(F95), F95&lt;&gt;E95), "_" &amp; TEXT(F95, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C95),"arith_" &amp; INDEX(Operations[],J95,2) &amp; "_g" &amp; TEXT(C95, "00") &amp; "_" &amp; TEXT(D95, "00") &amp; "_o" &amp; TEXT(E95, "00") &amp; IF(AND(ISNUMBER(F95), F95&gt;E95), "_" &amp; TEXT(F95, "00"), ""), "")</f>
         <v>arith_add_g09_00_o05_06</v>
       </c>
       <c r="B95" t="str">
@@ -4392,7 +4402,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="str">
-        <f>IF(ISNUMBER(C96),"arith_" &amp; INDEX(Operations[],J96,2) &amp; "_g" &amp; TEXT(C96, "00") &amp; "_" &amp; TEXT(D96, "00") &amp; "_o" &amp; TEXT(E96, "00") &amp; IF(AND(ISNUMBER(F96), F96&lt;&gt;E96), "_" &amp; TEXT(F96, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C96),"arith_" &amp; INDEX(Operations[],J96,2) &amp; "_g" &amp; TEXT(C96, "00") &amp; "_" &amp; TEXT(D96, "00") &amp; "_o" &amp; TEXT(E96, "00") &amp; IF(AND(ISNUMBER(F96), F96&gt;E96), "_" &amp; TEXT(F96, "00"), ""), "")</f>
         <v>arith_add_g09_00_o06_07</v>
       </c>
       <c r="B96" t="str">
@@ -4434,7 +4444,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="str">
-        <f>IF(ISNUMBER(C97),"arith_" &amp; INDEX(Operations[],J97,2) &amp; "_g" &amp; TEXT(C97, "00") &amp; "_" &amp; TEXT(D97, "00") &amp; "_o" &amp; TEXT(E97, "00") &amp; IF(AND(ISNUMBER(F97), F97&lt;&gt;E97), "_" &amp; TEXT(F97, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C97),"arith_" &amp; INDEX(Operations[],J97,2) &amp; "_g" &amp; TEXT(C97, "00") &amp; "_" &amp; TEXT(D97, "00") &amp; "_o" &amp; TEXT(E97, "00") &amp; IF(AND(ISNUMBER(F97), F97&gt;E97), "_" &amp; TEXT(F97, "00"), ""), "")</f>
         <v>arith_add_g09_00_o07_08</v>
       </c>
       <c r="B97" t="str">
@@ -4476,7 +4486,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="str">
-        <f>IF(ISNUMBER(C98),"arith_" &amp; INDEX(Operations[],J98,2) &amp; "_g" &amp; TEXT(C98, "00") &amp; "_" &amp; TEXT(D98, "00") &amp; "_o" &amp; TEXT(E98, "00") &amp; IF(AND(ISNUMBER(F98), F98&lt;&gt;E98), "_" &amp; TEXT(F98, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C98),"arith_" &amp; INDEX(Operations[],J98,2) &amp; "_g" &amp; TEXT(C98, "00") &amp; "_" &amp; TEXT(D98, "00") &amp; "_o" &amp; TEXT(E98, "00") &amp; IF(AND(ISNUMBER(F98), F98&gt;E98), "_" &amp; TEXT(F98, "00"), ""), "")</f>
         <v>arith_add_g09_00_o08_09</v>
       </c>
       <c r="B98" t="str">
@@ -4518,7 +4528,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="str">
-        <f>IF(ISNUMBER(C99),"arith_" &amp; INDEX(Operations[],J99,2) &amp; "_g" &amp; TEXT(C99, "00") &amp; "_" &amp; TEXT(D99, "00") &amp; "_o" &amp; TEXT(E99, "00") &amp; IF(AND(ISNUMBER(F99), F99&lt;&gt;E99), "_" &amp; TEXT(F99, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C99),"arith_" &amp; INDEX(Operations[],J99,2) &amp; "_g" &amp; TEXT(C99, "00") &amp; "_" &amp; TEXT(D99, "00") &amp; "_o" &amp; TEXT(E99, "00") &amp; IF(AND(ISNUMBER(F99), F99&gt;E99), "_" &amp; TEXT(F99, "00"), ""), "")</f>
         <v>arith_add_g09_00_o09_10</v>
       </c>
       <c r="B99" t="str">
@@ -4560,7 +4570,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="str">
-        <f>IF(ISNUMBER(C100),"arith_" &amp; INDEX(Operations[],J100,2) &amp; "_g" &amp; TEXT(C100, "00") &amp; "_" &amp; TEXT(D100, "00") &amp; "_o" &amp; TEXT(E100, "00") &amp; IF(AND(ISNUMBER(F100), F100&lt;&gt;E100), "_" &amp; TEXT(F100, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C100),"arith_" &amp; INDEX(Operations[],J100,2) &amp; "_g" &amp; TEXT(C100, "00") &amp; "_" &amp; TEXT(D100, "00") &amp; "_o" &amp; TEXT(E100, "00") &amp; IF(AND(ISNUMBER(F100), F100&gt;E100), "_" &amp; TEXT(F100, "00"), ""), "")</f>
         <v>arith_add_g09_00_o10</v>
       </c>
       <c r="B100" t="str">
@@ -4602,7 +4612,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="str">
-        <f>IF(ISNUMBER(C101),"arith_" &amp; INDEX(Operations[],J101,2) &amp; "_g" &amp; TEXT(C101, "00") &amp; "_" &amp; TEXT(D101, "00") &amp; "_o" &amp; TEXT(E101, "00") &amp; IF(AND(ISNUMBER(F101), F101&lt;&gt;E101), "_" &amp; TEXT(F101, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C101),"arith_" &amp; INDEX(Operations[],J101,2) &amp; "_g" &amp; TEXT(C101, "00") &amp; "_" &amp; TEXT(D101, "00") &amp; "_o" &amp; TEXT(E101, "00") &amp; IF(AND(ISNUMBER(F101), F101&gt;E101), "_" &amp; TEXT(F101, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B101" t="str">
@@ -4644,7 +4654,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="str">
-        <f>IF(ISNUMBER(C102),"arith_" &amp; INDEX(Operations[],J102,2) &amp; "_g" &amp; TEXT(C102, "00") &amp; "_" &amp; TEXT(D102, "00") &amp; "_o" &amp; TEXT(E102, "00") &amp; IF(AND(ISNUMBER(F102), F102&lt;&gt;E102), "_" &amp; TEXT(F102, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C102),"arith_" &amp; INDEX(Operations[],J102,2) &amp; "_g" &amp; TEXT(C102, "00") &amp; "_" &amp; TEXT(D102, "00") &amp; "_o" &amp; TEXT(E102, "00") &amp; IF(AND(ISNUMBER(F102), F102&gt;E102), "_" &amp; TEXT(F102, "00"), ""), "")</f>
         <v>arith_add_g10_00_o01_02</v>
       </c>
       <c r="B102" t="str">
@@ -4686,7 +4696,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="str">
-        <f>IF(ISNUMBER(C103),"arith_" &amp; INDEX(Operations[],J103,2) &amp; "_g" &amp; TEXT(C103, "00") &amp; "_" &amp; TEXT(D103, "00") &amp; "_o" &amp; TEXT(E103, "00") &amp; IF(AND(ISNUMBER(F103), F103&lt;&gt;E103), "_" &amp; TEXT(F103, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C103),"arith_" &amp; INDEX(Operations[],J103,2) &amp; "_g" &amp; TEXT(C103, "00") &amp; "_" &amp; TEXT(D103, "00") &amp; "_o" &amp; TEXT(E103, "00") &amp; IF(AND(ISNUMBER(F103), F103&gt;E103), "_" &amp; TEXT(F103, "00"), ""), "")</f>
         <v>arith_add_g10_00_o02_03</v>
       </c>
       <c r="B103" t="str">
@@ -4728,7 +4738,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="str">
-        <f>IF(ISNUMBER(C104),"arith_" &amp; INDEX(Operations[],J104,2) &amp; "_g" &amp; TEXT(C104, "00") &amp; "_" &amp; TEXT(D104, "00") &amp; "_o" &amp; TEXT(E104, "00") &amp; IF(AND(ISNUMBER(F104), F104&lt;&gt;E104), "_" &amp; TEXT(F104, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C104),"arith_" &amp; INDEX(Operations[],J104,2) &amp; "_g" &amp; TEXT(C104, "00") &amp; "_" &amp; TEXT(D104, "00") &amp; "_o" &amp; TEXT(E104, "00") &amp; IF(AND(ISNUMBER(F104), F104&gt;E104), "_" &amp; TEXT(F104, "00"), ""), "")</f>
         <v>arith_add_g10_00_o03_04</v>
       </c>
       <c r="B104" t="str">
@@ -4770,7 +4780,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="str">
-        <f>IF(ISNUMBER(C105),"arith_" &amp; INDEX(Operations[],J105,2) &amp; "_g" &amp; TEXT(C105, "00") &amp; "_" &amp; TEXT(D105, "00") &amp; "_o" &amp; TEXT(E105, "00") &amp; IF(AND(ISNUMBER(F105), F105&lt;&gt;E105), "_" &amp; TEXT(F105, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C105),"arith_" &amp; INDEX(Operations[],J105,2) &amp; "_g" &amp; TEXT(C105, "00") &amp; "_" &amp; TEXT(D105, "00") &amp; "_o" &amp; TEXT(E105, "00") &amp; IF(AND(ISNUMBER(F105), F105&gt;E105), "_" &amp; TEXT(F105, "00"), ""), "")</f>
         <v>arith_add_g10_00_o04_05</v>
       </c>
       <c r="B105" t="str">
@@ -4812,7 +4822,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="str">
-        <f>IF(ISNUMBER(C106),"arith_" &amp; INDEX(Operations[],J106,2) &amp; "_g" &amp; TEXT(C106, "00") &amp; "_" &amp; TEXT(D106, "00") &amp; "_o" &amp; TEXT(E106, "00") &amp; IF(AND(ISNUMBER(F106), F106&lt;&gt;E106), "_" &amp; TEXT(F106, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C106),"arith_" &amp; INDEX(Operations[],J106,2) &amp; "_g" &amp; TEXT(C106, "00") &amp; "_" &amp; TEXT(D106, "00") &amp; "_o" &amp; TEXT(E106, "00") &amp; IF(AND(ISNUMBER(F106), F106&gt;E106), "_" &amp; TEXT(F106, "00"), ""), "")</f>
         <v>arith_add_g10_00_o05_06</v>
       </c>
       <c r="B106" t="str">
@@ -4854,7 +4864,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="str">
-        <f>IF(ISNUMBER(C107),"arith_" &amp; INDEX(Operations[],J107,2) &amp; "_g" &amp; TEXT(C107, "00") &amp; "_" &amp; TEXT(D107, "00") &amp; "_o" &amp; TEXT(E107, "00") &amp; IF(AND(ISNUMBER(F107), F107&lt;&gt;E107), "_" &amp; TEXT(F107, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C107),"arith_" &amp; INDEX(Operations[],J107,2) &amp; "_g" &amp; TEXT(C107, "00") &amp; "_" &amp; TEXT(D107, "00") &amp; "_o" &amp; TEXT(E107, "00") &amp; IF(AND(ISNUMBER(F107), F107&gt;E107), "_" &amp; TEXT(F107, "00"), ""), "")</f>
         <v>arith_add_g10_00_o06_07</v>
       </c>
       <c r="B107" t="str">
@@ -4896,7 +4906,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="str">
-        <f>IF(ISNUMBER(C108),"arith_" &amp; INDEX(Operations[],J108,2) &amp; "_g" &amp; TEXT(C108, "00") &amp; "_" &amp; TEXT(D108, "00") &amp; "_o" &amp; TEXT(E108, "00") &amp; IF(AND(ISNUMBER(F108), F108&lt;&gt;E108), "_" &amp; TEXT(F108, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C108),"arith_" &amp; INDEX(Operations[],J108,2) &amp; "_g" &amp; TEXT(C108, "00") &amp; "_" &amp; TEXT(D108, "00") &amp; "_o" &amp; TEXT(E108, "00") &amp; IF(AND(ISNUMBER(F108), F108&gt;E108), "_" &amp; TEXT(F108, "00"), ""), "")</f>
         <v>arith_add_g10_00_o07_08</v>
       </c>
       <c r="B108" t="str">
@@ -4938,7 +4948,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="str">
-        <f>IF(ISNUMBER(C109),"arith_" &amp; INDEX(Operations[],J109,2) &amp; "_g" &amp; TEXT(C109, "00") &amp; "_" &amp; TEXT(D109, "00") &amp; "_o" &amp; TEXT(E109, "00") &amp; IF(AND(ISNUMBER(F109), F109&lt;&gt;E109), "_" &amp; TEXT(F109, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C109),"arith_" &amp; INDEX(Operations[],J109,2) &amp; "_g" &amp; TEXT(C109, "00") &amp; "_" &amp; TEXT(D109, "00") &amp; "_o" &amp; TEXT(E109, "00") &amp; IF(AND(ISNUMBER(F109), F109&gt;E109), "_" &amp; TEXT(F109, "00"), ""), "")</f>
         <v>arith_add_g10_00_o08_09</v>
       </c>
       <c r="B109" t="str">
@@ -4980,7 +4990,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
-        <f>IF(ISNUMBER(C110),"arith_" &amp; INDEX(Operations[],J110,2) &amp; "_g" &amp; TEXT(C110, "00") &amp; "_" &amp; TEXT(D110, "00") &amp; "_o" &amp; TEXT(E110, "00") &amp; IF(AND(ISNUMBER(F110), F110&lt;&gt;E110), "_" &amp; TEXT(F110, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C110),"arith_" &amp; INDEX(Operations[],J110,2) &amp; "_g" &amp; TEXT(C110, "00") &amp; "_" &amp; TEXT(D110, "00") &amp; "_o" &amp; TEXT(E110, "00") &amp; IF(AND(ISNUMBER(F110), F110&gt;E110), "_" &amp; TEXT(F110, "00"), ""), "")</f>
         <v>arith_add_g10_00_o09_10</v>
       </c>
       <c r="B110" t="str">
@@ -5022,7 +5032,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
-        <f>IF(ISNUMBER(C111),"arith_" &amp; INDEX(Operations[],J111,2) &amp; "_g" &amp; TEXT(C111, "00") &amp; "_" &amp; TEXT(D111, "00") &amp; "_o" &amp; TEXT(E111, "00") &amp; IF(AND(ISNUMBER(F111), F111&lt;&gt;E111), "_" &amp; TEXT(F111, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C111),"arith_" &amp; INDEX(Operations[],J111,2) &amp; "_g" &amp; TEXT(C111, "00") &amp; "_" &amp; TEXT(D111, "00") &amp; "_o" &amp; TEXT(E111, "00") &amp; IF(AND(ISNUMBER(F111), F111&gt;E111), "_" &amp; TEXT(F111, "00"), ""), "")</f>
         <v>arith_add_g10_00_o10</v>
       </c>
       <c r="B111" t="str">
@@ -5064,7 +5074,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
-        <f>IF(ISNUMBER(C112),"arith_" &amp; INDEX(Operations[],J112,2) &amp; "_g" &amp; TEXT(C112, "00") &amp; "_" &amp; TEXT(D112, "00") &amp; "_o" &amp; TEXT(E112, "00") &amp; IF(AND(ISNUMBER(F112), F112&lt;&gt;E112), "_" &amp; TEXT(F112, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C112),"arith_" &amp; INDEX(Operations[],J112,2) &amp; "_g" &amp; TEXT(C112, "00") &amp; "_" &amp; TEXT(D112, "00") &amp; "_o" &amp; TEXT(E112, "00") &amp; IF(AND(ISNUMBER(F112), F112&gt;E112), "_" &amp; TEXT(F112, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B112" t="str">
@@ -5106,7 +5116,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
-        <f>IF(ISNUMBER(C113),"arith_" &amp; INDEX(Operations[],J113,2) &amp; "_g" &amp; TEXT(C113, "00") &amp; "_" &amp; TEXT(D113, "00") &amp; "_o" &amp; TEXT(E113, "00") &amp; IF(AND(ISNUMBER(F113), F113&lt;&gt;E113), "_" &amp; TEXT(F113, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C113),"arith_" &amp; INDEX(Operations[],J113,2) &amp; "_g" &amp; TEXT(C113, "00") &amp; "_" &amp; TEXT(D113, "00") &amp; "_o" &amp; TEXT(E113, "00") &amp; IF(AND(ISNUMBER(F113), F113&gt;E113), "_" &amp; TEXT(F113, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o01_02</v>
       </c>
       <c r="B113" t="str">
@@ -5148,7 +5158,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
-        <f>IF(ISNUMBER(C114),"arith_" &amp; INDEX(Operations[],J114,2) &amp; "_g" &amp; TEXT(C114, "00") &amp; "_" &amp; TEXT(D114, "00") &amp; "_o" &amp; TEXT(E114, "00") &amp; IF(AND(ISNUMBER(F114), F114&lt;&gt;E114), "_" &amp; TEXT(F114, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C114),"arith_" &amp; INDEX(Operations[],J114,2) &amp; "_g" &amp; TEXT(C114, "00") &amp; "_" &amp; TEXT(D114, "00") &amp; "_o" &amp; TEXT(E114, "00") &amp; IF(AND(ISNUMBER(F114), F114&gt;E114), "_" &amp; TEXT(F114, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o02_03</v>
       </c>
       <c r="B114" t="str">
@@ -5190,7 +5200,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
-        <f>IF(ISNUMBER(C115),"arith_" &amp; INDEX(Operations[],J115,2) &amp; "_g" &amp; TEXT(C115, "00") &amp; "_" &amp; TEXT(D115, "00") &amp; "_o" &amp; TEXT(E115, "00") &amp; IF(AND(ISNUMBER(F115), F115&lt;&gt;E115), "_" &amp; TEXT(F115, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C115),"arith_" &amp; INDEX(Operations[],J115,2) &amp; "_g" &amp; TEXT(C115, "00") &amp; "_" &amp; TEXT(D115, "00") &amp; "_o" &amp; TEXT(E115, "00") &amp; IF(AND(ISNUMBER(F115), F115&gt;E115), "_" &amp; TEXT(F115, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o03_04</v>
       </c>
       <c r="B115" t="str">
@@ -5232,7 +5242,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="str">
-        <f>IF(ISNUMBER(C116),"arith_" &amp; INDEX(Operations[],J116,2) &amp; "_g" &amp; TEXT(C116, "00") &amp; "_" &amp; TEXT(D116, "00") &amp; "_o" &amp; TEXT(E116, "00") &amp; IF(AND(ISNUMBER(F116), F116&lt;&gt;E116), "_" &amp; TEXT(F116, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C116),"arith_" &amp; INDEX(Operations[],J116,2) &amp; "_g" &amp; TEXT(C116, "00") &amp; "_" &amp; TEXT(D116, "00") &amp; "_o" &amp; TEXT(E116, "00") &amp; IF(AND(ISNUMBER(F116), F116&gt;E116), "_" &amp; TEXT(F116, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o04_05</v>
       </c>
       <c r="B116" t="str">
@@ -5274,7 +5284,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="str">
-        <f>IF(ISNUMBER(C117),"arith_" &amp; INDEX(Operations[],J117,2) &amp; "_g" &amp; TEXT(C117, "00") &amp; "_" &amp; TEXT(D117, "00") &amp; "_o" &amp; TEXT(E117, "00") &amp; IF(AND(ISNUMBER(F117), F117&lt;&gt;E117), "_" &amp; TEXT(F117, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C117),"arith_" &amp; INDEX(Operations[],J117,2) &amp; "_g" &amp; TEXT(C117, "00") &amp; "_" &amp; TEXT(D117, "00") &amp; "_o" &amp; TEXT(E117, "00") &amp; IF(AND(ISNUMBER(F117), F117&gt;E117), "_" &amp; TEXT(F117, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o05_06</v>
       </c>
       <c r="B117" t="str">
@@ -5316,7 +5326,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="str">
-        <f>IF(ISNUMBER(C118),"arith_" &amp; INDEX(Operations[],J118,2) &amp; "_g" &amp; TEXT(C118, "00") &amp; "_" &amp; TEXT(D118, "00") &amp; "_o" &amp; TEXT(E118, "00") &amp; IF(AND(ISNUMBER(F118), F118&lt;&gt;E118), "_" &amp; TEXT(F118, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C118),"arith_" &amp; INDEX(Operations[],J118,2) &amp; "_g" &amp; TEXT(C118, "00") &amp; "_" &amp; TEXT(D118, "00") &amp; "_o" &amp; TEXT(E118, "00") &amp; IF(AND(ISNUMBER(F118), F118&gt;E118), "_" &amp; TEXT(F118, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o06_07</v>
       </c>
       <c r="B118" t="str">
@@ -5358,7 +5368,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="str">
-        <f>IF(ISNUMBER(C119),"arith_" &amp; INDEX(Operations[],J119,2) &amp; "_g" &amp; TEXT(C119, "00") &amp; "_" &amp; TEXT(D119, "00") &amp; "_o" &amp; TEXT(E119, "00") &amp; IF(AND(ISNUMBER(F119), F119&lt;&gt;E119), "_" &amp; TEXT(F119, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C119),"arith_" &amp; INDEX(Operations[],J119,2) &amp; "_g" &amp; TEXT(C119, "00") &amp; "_" &amp; TEXT(D119, "00") &amp; "_o" &amp; TEXT(E119, "00") &amp; IF(AND(ISNUMBER(F119), F119&gt;E119), "_" &amp; TEXT(F119, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o07_08</v>
       </c>
       <c r="B119" t="str">
@@ -5400,7 +5410,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="str">
-        <f>IF(ISNUMBER(C120),"arith_" &amp; INDEX(Operations[],J120,2) &amp; "_g" &amp; TEXT(C120, "00") &amp; "_" &amp; TEXT(D120, "00") &amp; "_o" &amp; TEXT(E120, "00") &amp; IF(AND(ISNUMBER(F120), F120&lt;&gt;E120), "_" &amp; TEXT(F120, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C120),"arith_" &amp; INDEX(Operations[],J120,2) &amp; "_g" &amp; TEXT(C120, "00") &amp; "_" &amp; TEXT(D120, "00") &amp; "_o" &amp; TEXT(E120, "00") &amp; IF(AND(ISNUMBER(F120), F120&gt;E120), "_" &amp; TEXT(F120, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o08_09</v>
       </c>
       <c r="B120" t="str">
@@ -5442,7 +5452,7 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="str">
-        <f>IF(ISNUMBER(C121),"arith_" &amp; INDEX(Operations[],J121,2) &amp; "_g" &amp; TEXT(C121, "00") &amp; "_" &amp; TEXT(D121, "00") &amp; "_o" &amp; TEXT(E121, "00") &amp; IF(AND(ISNUMBER(F121), F121&lt;&gt;E121), "_" &amp; TEXT(F121, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C121),"arith_" &amp; INDEX(Operations[],J121,2) &amp; "_g" &amp; TEXT(C121, "00") &amp; "_" &amp; TEXT(D121, "00") &amp; "_o" &amp; TEXT(E121, "00") &amp; IF(AND(ISNUMBER(F121), F121&gt;E121), "_" &amp; TEXT(F121, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o09_10</v>
       </c>
       <c r="B121" t="str">
@@ -5484,7 +5494,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="str">
-        <f>IF(ISNUMBER(C122),"arith_" &amp; INDEX(Operations[],J122,2) &amp; "_g" &amp; TEXT(C122, "00") &amp; "_" &amp; TEXT(D122, "00") &amp; "_o" &amp; TEXT(E122, "00") &amp; IF(AND(ISNUMBER(F122), F122&lt;&gt;E122), "_" &amp; TEXT(F122, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C122),"arith_" &amp; INDEX(Operations[],J122,2) &amp; "_g" &amp; TEXT(C122, "00") &amp; "_" &amp; TEXT(D122, "00") &amp; "_o" &amp; TEXT(E122, "00") &amp; IF(AND(ISNUMBER(F122), F122&gt;E122), "_" &amp; TEXT(F122, "00"), ""), "")</f>
         <v>arith_sub_g01_00_o10</v>
       </c>
       <c r="B122" t="str">
@@ -5526,7 +5536,7 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="str">
-        <f>IF(ISNUMBER(C123),"arith_" &amp; INDEX(Operations[],J123,2) &amp; "_g" &amp; TEXT(C123, "00") &amp; "_" &amp; TEXT(D123, "00") &amp; "_o" &amp; TEXT(E123, "00") &amp; IF(AND(ISNUMBER(F123), F123&lt;&gt;E123), "_" &amp; TEXT(F123, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C123),"arith_" &amp; INDEX(Operations[],J123,2) &amp; "_g" &amp; TEXT(C123, "00") &amp; "_" &amp; TEXT(D123, "00") &amp; "_o" &amp; TEXT(E123, "00") &amp; IF(AND(ISNUMBER(F123), F123&gt;E123), "_" &amp; TEXT(F123, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B123" t="str">
@@ -5568,7 +5578,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="str">
-        <f>IF(ISNUMBER(C124),"arith_" &amp; INDEX(Operations[],J124,2) &amp; "_g" &amp; TEXT(C124, "00") &amp; "_" &amp; TEXT(D124, "00") &amp; "_o" &amp; TEXT(E124, "00") &amp; IF(AND(ISNUMBER(F124), F124&lt;&gt;E124), "_" &amp; TEXT(F124, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C124),"arith_" &amp; INDEX(Operations[],J124,2) &amp; "_g" &amp; TEXT(C124, "00") &amp; "_" &amp; TEXT(D124, "00") &amp; "_o" &amp; TEXT(E124, "00") &amp; IF(AND(ISNUMBER(F124), F124&gt;E124), "_" &amp; TEXT(F124, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o01_02</v>
       </c>
       <c r="B124" t="str">
@@ -5610,7 +5620,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
-        <f>IF(ISNUMBER(C125),"arith_" &amp; INDEX(Operations[],J125,2) &amp; "_g" &amp; TEXT(C125, "00") &amp; "_" &amp; TEXT(D125, "00") &amp; "_o" &amp; TEXT(E125, "00") &amp; IF(AND(ISNUMBER(F125), F125&lt;&gt;E125), "_" &amp; TEXT(F125, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C125),"arith_" &amp; INDEX(Operations[],J125,2) &amp; "_g" &amp; TEXT(C125, "00") &amp; "_" &amp; TEXT(D125, "00") &amp; "_o" &amp; TEXT(E125, "00") &amp; IF(AND(ISNUMBER(F125), F125&gt;E125), "_" &amp; TEXT(F125, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o02_03</v>
       </c>
       <c r="B125" t="str">
@@ -5652,7 +5662,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
-        <f>IF(ISNUMBER(C126),"arith_" &amp; INDEX(Operations[],J126,2) &amp; "_g" &amp; TEXT(C126, "00") &amp; "_" &amp; TEXT(D126, "00") &amp; "_o" &amp; TEXT(E126, "00") &amp; IF(AND(ISNUMBER(F126), F126&lt;&gt;E126), "_" &amp; TEXT(F126, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C126),"arith_" &amp; INDEX(Operations[],J126,2) &amp; "_g" &amp; TEXT(C126, "00") &amp; "_" &amp; TEXT(D126, "00") &amp; "_o" &amp; TEXT(E126, "00") &amp; IF(AND(ISNUMBER(F126), F126&gt;E126), "_" &amp; TEXT(F126, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o03_04</v>
       </c>
       <c r="B126" t="str">
@@ -5694,7 +5704,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
-        <f>IF(ISNUMBER(C127),"arith_" &amp; INDEX(Operations[],J127,2) &amp; "_g" &amp; TEXT(C127, "00") &amp; "_" &amp; TEXT(D127, "00") &amp; "_o" &amp; TEXT(E127, "00") &amp; IF(AND(ISNUMBER(F127), F127&lt;&gt;E127), "_" &amp; TEXT(F127, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C127),"arith_" &amp; INDEX(Operations[],J127,2) &amp; "_g" &amp; TEXT(C127, "00") &amp; "_" &amp; TEXT(D127, "00") &amp; "_o" &amp; TEXT(E127, "00") &amp; IF(AND(ISNUMBER(F127), F127&gt;E127), "_" &amp; TEXT(F127, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o04_05</v>
       </c>
       <c r="B127" t="str">
@@ -5736,7 +5746,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
-        <f>IF(ISNUMBER(C128),"arith_" &amp; INDEX(Operations[],J128,2) &amp; "_g" &amp; TEXT(C128, "00") &amp; "_" &amp; TEXT(D128, "00") &amp; "_o" &amp; TEXT(E128, "00") &amp; IF(AND(ISNUMBER(F128), F128&lt;&gt;E128), "_" &amp; TEXT(F128, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C128),"arith_" &amp; INDEX(Operations[],J128,2) &amp; "_g" &amp; TEXT(C128, "00") &amp; "_" &amp; TEXT(D128, "00") &amp; "_o" &amp; TEXT(E128, "00") &amp; IF(AND(ISNUMBER(F128), F128&gt;E128), "_" &amp; TEXT(F128, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o05_06</v>
       </c>
       <c r="B128" t="str">
@@ -5778,7 +5788,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
-        <f>IF(ISNUMBER(C129),"arith_" &amp; INDEX(Operations[],J129,2) &amp; "_g" &amp; TEXT(C129, "00") &amp; "_" &amp; TEXT(D129, "00") &amp; "_o" &amp; TEXT(E129, "00") &amp; IF(AND(ISNUMBER(F129), F129&lt;&gt;E129), "_" &amp; TEXT(F129, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C129),"arith_" &amp; INDEX(Operations[],J129,2) &amp; "_g" &amp; TEXT(C129, "00") &amp; "_" &amp; TEXT(D129, "00") &amp; "_o" &amp; TEXT(E129, "00") &amp; IF(AND(ISNUMBER(F129), F129&gt;E129), "_" &amp; TEXT(F129, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o06_07</v>
       </c>
       <c r="B129" t="str">
@@ -5820,7 +5830,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
-        <f>IF(ISNUMBER(C130),"arith_" &amp; INDEX(Operations[],J130,2) &amp; "_g" &amp; TEXT(C130, "00") &amp; "_" &amp; TEXT(D130, "00") &amp; "_o" &amp; TEXT(E130, "00") &amp; IF(AND(ISNUMBER(F130), F130&lt;&gt;E130), "_" &amp; TEXT(F130, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C130),"arith_" &amp; INDEX(Operations[],J130,2) &amp; "_g" &amp; TEXT(C130, "00") &amp; "_" &amp; TEXT(D130, "00") &amp; "_o" &amp; TEXT(E130, "00") &amp; IF(AND(ISNUMBER(F130), F130&gt;E130), "_" &amp; TEXT(F130, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o07_08</v>
       </c>
       <c r="B130" t="str">
@@ -5862,7 +5872,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="str">
-        <f>IF(ISNUMBER(C131),"arith_" &amp; INDEX(Operations[],J131,2) &amp; "_g" &amp; TEXT(C131, "00") &amp; "_" &amp; TEXT(D131, "00") &amp; "_o" &amp; TEXT(E131, "00") &amp; IF(AND(ISNUMBER(F131), F131&lt;&gt;E131), "_" &amp; TEXT(F131, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C131),"arith_" &amp; INDEX(Operations[],J131,2) &amp; "_g" &amp; TEXT(C131, "00") &amp; "_" &amp; TEXT(D131, "00") &amp; "_o" &amp; TEXT(E131, "00") &amp; IF(AND(ISNUMBER(F131), F131&gt;E131), "_" &amp; TEXT(F131, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o08_09</v>
       </c>
       <c r="B131" t="str">
@@ -5904,7 +5914,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="str">
-        <f>IF(ISNUMBER(C132),"arith_" &amp; INDEX(Operations[],J132,2) &amp; "_g" &amp; TEXT(C132, "00") &amp; "_" &amp; TEXT(D132, "00") &amp; "_o" &amp; TEXT(E132, "00") &amp; IF(AND(ISNUMBER(F132), F132&lt;&gt;E132), "_" &amp; TEXT(F132, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C132),"arith_" &amp; INDEX(Operations[],J132,2) &amp; "_g" &amp; TEXT(C132, "00") &amp; "_" &amp; TEXT(D132, "00") &amp; "_o" &amp; TEXT(E132, "00") &amp; IF(AND(ISNUMBER(F132), F132&gt;E132), "_" &amp; TEXT(F132, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o09_10</v>
       </c>
       <c r="B132" t="str">
@@ -5946,7 +5956,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="str">
-        <f>IF(ISNUMBER(C133),"arith_" &amp; INDEX(Operations[],J133,2) &amp; "_g" &amp; TEXT(C133, "00") &amp; "_" &amp; TEXT(D133, "00") &amp; "_o" &amp; TEXT(E133, "00") &amp; IF(AND(ISNUMBER(F133), F133&lt;&gt;E133), "_" &amp; TEXT(F133, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C133),"arith_" &amp; INDEX(Operations[],J133,2) &amp; "_g" &amp; TEXT(C133, "00") &amp; "_" &amp; TEXT(D133, "00") &amp; "_o" &amp; TEXT(E133, "00") &amp; IF(AND(ISNUMBER(F133), F133&gt;E133), "_" &amp; TEXT(F133, "00"), ""), "")</f>
         <v>arith_sub_g02_00_o10</v>
       </c>
       <c r="B133" t="str">
@@ -5988,7 +5998,7 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="str">
-        <f>IF(ISNUMBER(C134),"arith_" &amp; INDEX(Operations[],J134,2) &amp; "_g" &amp; TEXT(C134, "00") &amp; "_" &amp; TEXT(D134, "00") &amp; "_o" &amp; TEXT(E134, "00") &amp; IF(AND(ISNUMBER(F134), F134&lt;&gt;E134), "_" &amp; TEXT(F134, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C134),"arith_" &amp; INDEX(Operations[],J134,2) &amp; "_g" &amp; TEXT(C134, "00") &amp; "_" &amp; TEXT(D134, "00") &amp; "_o" &amp; TEXT(E134, "00") &amp; IF(AND(ISNUMBER(F134), F134&gt;E134), "_" &amp; TEXT(F134, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B134" t="str">
@@ -6030,7 +6040,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="str">
-        <f>IF(ISNUMBER(C135),"arith_" &amp; INDEX(Operations[],J135,2) &amp; "_g" &amp; TEXT(C135, "00") &amp; "_" &amp; TEXT(D135, "00") &amp; "_o" &amp; TEXT(E135, "00") &amp; IF(AND(ISNUMBER(F135), F135&lt;&gt;E135), "_" &amp; TEXT(F135, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C135),"arith_" &amp; INDEX(Operations[],J135,2) &amp; "_g" &amp; TEXT(C135, "00") &amp; "_" &amp; TEXT(D135, "00") &amp; "_o" &amp; TEXT(E135, "00") &amp; IF(AND(ISNUMBER(F135), F135&gt;E135), "_" &amp; TEXT(F135, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o01_02</v>
       </c>
       <c r="B135" t="str">
@@ -6072,7 +6082,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="str">
-        <f>IF(ISNUMBER(C136),"arith_" &amp; INDEX(Operations[],J136,2) &amp; "_g" &amp; TEXT(C136, "00") &amp; "_" &amp; TEXT(D136, "00") &amp; "_o" &amp; TEXT(E136, "00") &amp; IF(AND(ISNUMBER(F136), F136&lt;&gt;E136), "_" &amp; TEXT(F136, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C136),"arith_" &amp; INDEX(Operations[],J136,2) &amp; "_g" &amp; TEXT(C136, "00") &amp; "_" &amp; TEXT(D136, "00") &amp; "_o" &amp; TEXT(E136, "00") &amp; IF(AND(ISNUMBER(F136), F136&gt;E136), "_" &amp; TEXT(F136, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o02_03</v>
       </c>
       <c r="B136" t="str">
@@ -6114,7 +6124,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="str">
-        <f>IF(ISNUMBER(C137),"arith_" &amp; INDEX(Operations[],J137,2) &amp; "_g" &amp; TEXT(C137, "00") &amp; "_" &amp; TEXT(D137, "00") &amp; "_o" &amp; TEXT(E137, "00") &amp; IF(AND(ISNUMBER(F137), F137&lt;&gt;E137), "_" &amp; TEXT(F137, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C137),"arith_" &amp; INDEX(Operations[],J137,2) &amp; "_g" &amp; TEXT(C137, "00") &amp; "_" &amp; TEXT(D137, "00") &amp; "_o" &amp; TEXT(E137, "00") &amp; IF(AND(ISNUMBER(F137), F137&gt;E137), "_" &amp; TEXT(F137, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o03_04</v>
       </c>
       <c r="B137" t="str">
@@ -6156,7 +6166,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="str">
-        <f>IF(ISNUMBER(C138),"arith_" &amp; INDEX(Operations[],J138,2) &amp; "_g" &amp; TEXT(C138, "00") &amp; "_" &amp; TEXT(D138, "00") &amp; "_o" &amp; TEXT(E138, "00") &amp; IF(AND(ISNUMBER(F138), F138&lt;&gt;E138), "_" &amp; TEXT(F138, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C138),"arith_" &amp; INDEX(Operations[],J138,2) &amp; "_g" &amp; TEXT(C138, "00") &amp; "_" &amp; TEXT(D138, "00") &amp; "_o" &amp; TEXT(E138, "00") &amp; IF(AND(ISNUMBER(F138), F138&gt;E138), "_" &amp; TEXT(F138, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o04_05</v>
       </c>
       <c r="B138" t="str">
@@ -6198,7 +6208,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="str">
-        <f>IF(ISNUMBER(C139),"arith_" &amp; INDEX(Operations[],J139,2) &amp; "_g" &amp; TEXT(C139, "00") &amp; "_" &amp; TEXT(D139, "00") &amp; "_o" &amp; TEXT(E139, "00") &amp; IF(AND(ISNUMBER(F139), F139&lt;&gt;E139), "_" &amp; TEXT(F139, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C139),"arith_" &amp; INDEX(Operations[],J139,2) &amp; "_g" &amp; TEXT(C139, "00") &amp; "_" &amp; TEXT(D139, "00") &amp; "_o" &amp; TEXT(E139, "00") &amp; IF(AND(ISNUMBER(F139), F139&gt;E139), "_" &amp; TEXT(F139, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o05_06</v>
       </c>
       <c r="B139" t="str">
@@ -6240,7 +6250,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="str">
-        <f>IF(ISNUMBER(C140),"arith_" &amp; INDEX(Operations[],J140,2) &amp; "_g" &amp; TEXT(C140, "00") &amp; "_" &amp; TEXT(D140, "00") &amp; "_o" &amp; TEXT(E140, "00") &amp; IF(AND(ISNUMBER(F140), F140&lt;&gt;E140), "_" &amp; TEXT(F140, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C140),"arith_" &amp; INDEX(Operations[],J140,2) &amp; "_g" &amp; TEXT(C140, "00") &amp; "_" &amp; TEXT(D140, "00") &amp; "_o" &amp; TEXT(E140, "00") &amp; IF(AND(ISNUMBER(F140), F140&gt;E140), "_" &amp; TEXT(F140, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o06_07</v>
       </c>
       <c r="B140" t="str">
@@ -6282,7 +6292,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="str">
-        <f>IF(ISNUMBER(C141),"arith_" &amp; INDEX(Operations[],J141,2) &amp; "_g" &amp; TEXT(C141, "00") &amp; "_" &amp; TEXT(D141, "00") &amp; "_o" &amp; TEXT(E141, "00") &amp; IF(AND(ISNUMBER(F141), F141&lt;&gt;E141), "_" &amp; TEXT(F141, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C141),"arith_" &amp; INDEX(Operations[],J141,2) &amp; "_g" &amp; TEXT(C141, "00") &amp; "_" &amp; TEXT(D141, "00") &amp; "_o" &amp; TEXT(E141, "00") &amp; IF(AND(ISNUMBER(F141), F141&gt;E141), "_" &amp; TEXT(F141, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o07_08</v>
       </c>
       <c r="B141" t="str">
@@ -6324,7 +6334,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="str">
-        <f>IF(ISNUMBER(C142),"arith_" &amp; INDEX(Operations[],J142,2) &amp; "_g" &amp; TEXT(C142, "00") &amp; "_" &amp; TEXT(D142, "00") &amp; "_o" &amp; TEXT(E142, "00") &amp; IF(AND(ISNUMBER(F142), F142&lt;&gt;E142), "_" &amp; TEXT(F142, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C142),"arith_" &amp; INDEX(Operations[],J142,2) &amp; "_g" &amp; TEXT(C142, "00") &amp; "_" &amp; TEXT(D142, "00") &amp; "_o" &amp; TEXT(E142, "00") &amp; IF(AND(ISNUMBER(F142), F142&gt;E142), "_" &amp; TEXT(F142, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o08_09</v>
       </c>
       <c r="B142" t="str">
@@ -6366,7 +6376,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="str">
-        <f>IF(ISNUMBER(C143),"arith_" &amp; INDEX(Operations[],J143,2) &amp; "_g" &amp; TEXT(C143, "00") &amp; "_" &amp; TEXT(D143, "00") &amp; "_o" &amp; TEXT(E143, "00") &amp; IF(AND(ISNUMBER(F143), F143&lt;&gt;E143), "_" &amp; TEXT(F143, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C143),"arith_" &amp; INDEX(Operations[],J143,2) &amp; "_g" &amp; TEXT(C143, "00") &amp; "_" &amp; TEXT(D143, "00") &amp; "_o" &amp; TEXT(E143, "00") &amp; IF(AND(ISNUMBER(F143), F143&gt;E143), "_" &amp; TEXT(F143, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o09_10</v>
       </c>
       <c r="B143" t="str">
@@ -6408,7 +6418,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="str">
-        <f>IF(ISNUMBER(C144),"arith_" &amp; INDEX(Operations[],J144,2) &amp; "_g" &amp; TEXT(C144, "00") &amp; "_" &amp; TEXT(D144, "00") &amp; "_o" &amp; TEXT(E144, "00") &amp; IF(AND(ISNUMBER(F144), F144&lt;&gt;E144), "_" &amp; TEXT(F144, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C144),"arith_" &amp; INDEX(Operations[],J144,2) &amp; "_g" &amp; TEXT(C144, "00") &amp; "_" &amp; TEXT(D144, "00") &amp; "_o" &amp; TEXT(E144, "00") &amp; IF(AND(ISNUMBER(F144), F144&gt;E144), "_" &amp; TEXT(F144, "00"), ""), "")</f>
         <v>arith_sub_g03_00_o10</v>
       </c>
       <c r="B144" t="str">
@@ -6450,7 +6460,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="str">
-        <f>IF(ISNUMBER(C145),"arith_" &amp; INDEX(Operations[],J145,2) &amp; "_g" &amp; TEXT(C145, "00") &amp; "_" &amp; TEXT(D145, "00") &amp; "_o" &amp; TEXT(E145, "00") &amp; IF(AND(ISNUMBER(F145), F145&lt;&gt;E145), "_" &amp; TEXT(F145, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C145),"arith_" &amp; INDEX(Operations[],J145,2) &amp; "_g" &amp; TEXT(C145, "00") &amp; "_" &amp; TEXT(D145, "00") &amp; "_o" &amp; TEXT(E145, "00") &amp; IF(AND(ISNUMBER(F145), F145&gt;E145), "_" &amp; TEXT(F145, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B145" t="str">
@@ -6492,7 +6502,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="str">
-        <f>IF(ISNUMBER(C146),"arith_" &amp; INDEX(Operations[],J146,2) &amp; "_g" &amp; TEXT(C146, "00") &amp; "_" &amp; TEXT(D146, "00") &amp; "_o" &amp; TEXT(E146, "00") &amp; IF(AND(ISNUMBER(F146), F146&lt;&gt;E146), "_" &amp; TEXT(F146, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C146),"arith_" &amp; INDEX(Operations[],J146,2) &amp; "_g" &amp; TEXT(C146, "00") &amp; "_" &amp; TEXT(D146, "00") &amp; "_o" &amp; TEXT(E146, "00") &amp; IF(AND(ISNUMBER(F146), F146&gt;E146), "_" &amp; TEXT(F146, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o01_02</v>
       </c>
       <c r="B146" t="str">
@@ -6534,7 +6544,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="str">
-        <f>IF(ISNUMBER(C147),"arith_" &amp; INDEX(Operations[],J147,2) &amp; "_g" &amp; TEXT(C147, "00") &amp; "_" &amp; TEXT(D147, "00") &amp; "_o" &amp; TEXT(E147, "00") &amp; IF(AND(ISNUMBER(F147), F147&lt;&gt;E147), "_" &amp; TEXT(F147, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C147),"arith_" &amp; INDEX(Operations[],J147,2) &amp; "_g" &amp; TEXT(C147, "00") &amp; "_" &amp; TEXT(D147, "00") &amp; "_o" &amp; TEXT(E147, "00") &amp; IF(AND(ISNUMBER(F147), F147&gt;E147), "_" &amp; TEXT(F147, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o02_03</v>
       </c>
       <c r="B147" t="str">
@@ -6576,7 +6586,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="str">
-        <f>IF(ISNUMBER(C148),"arith_" &amp; INDEX(Operations[],J148,2) &amp; "_g" &amp; TEXT(C148, "00") &amp; "_" &amp; TEXT(D148, "00") &amp; "_o" &amp; TEXT(E148, "00") &amp; IF(AND(ISNUMBER(F148), F148&lt;&gt;E148), "_" &amp; TEXT(F148, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C148),"arith_" &amp; INDEX(Operations[],J148,2) &amp; "_g" &amp; TEXT(C148, "00") &amp; "_" &amp; TEXT(D148, "00") &amp; "_o" &amp; TEXT(E148, "00") &amp; IF(AND(ISNUMBER(F148), F148&gt;E148), "_" &amp; TEXT(F148, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o03_04</v>
       </c>
       <c r="B148" t="str">
@@ -6618,7 +6628,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="str">
-        <f>IF(ISNUMBER(C149),"arith_" &amp; INDEX(Operations[],J149,2) &amp; "_g" &amp; TEXT(C149, "00") &amp; "_" &amp; TEXT(D149, "00") &amp; "_o" &amp; TEXT(E149, "00") &amp; IF(AND(ISNUMBER(F149), F149&lt;&gt;E149), "_" &amp; TEXT(F149, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C149),"arith_" &amp; INDEX(Operations[],J149,2) &amp; "_g" &amp; TEXT(C149, "00") &amp; "_" &amp; TEXT(D149, "00") &amp; "_o" &amp; TEXT(E149, "00") &amp; IF(AND(ISNUMBER(F149), F149&gt;E149), "_" &amp; TEXT(F149, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o04_05</v>
       </c>
       <c r="B149" t="str">
@@ -6660,7 +6670,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="str">
-        <f>IF(ISNUMBER(C150),"arith_" &amp; INDEX(Operations[],J150,2) &amp; "_g" &amp; TEXT(C150, "00") &amp; "_" &amp; TEXT(D150, "00") &amp; "_o" &amp; TEXT(E150, "00") &amp; IF(AND(ISNUMBER(F150), F150&lt;&gt;E150), "_" &amp; TEXT(F150, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C150),"arith_" &amp; INDEX(Operations[],J150,2) &amp; "_g" &amp; TEXT(C150, "00") &amp; "_" &amp; TEXT(D150, "00") &amp; "_o" &amp; TEXT(E150, "00") &amp; IF(AND(ISNUMBER(F150), F150&gt;E150), "_" &amp; TEXT(F150, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o05_06</v>
       </c>
       <c r="B150" t="str">
@@ -6702,7 +6712,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="str">
-        <f>IF(ISNUMBER(C151),"arith_" &amp; INDEX(Operations[],J151,2) &amp; "_g" &amp; TEXT(C151, "00") &amp; "_" &amp; TEXT(D151, "00") &amp; "_o" &amp; TEXT(E151, "00") &amp; IF(AND(ISNUMBER(F151), F151&lt;&gt;E151), "_" &amp; TEXT(F151, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C151),"arith_" &amp; INDEX(Operations[],J151,2) &amp; "_g" &amp; TEXT(C151, "00") &amp; "_" &amp; TEXT(D151, "00") &amp; "_o" &amp; TEXT(E151, "00") &amp; IF(AND(ISNUMBER(F151), F151&gt;E151), "_" &amp; TEXT(F151, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o06_07</v>
       </c>
       <c r="B151" t="str">
@@ -6744,7 +6754,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="str">
-        <f>IF(ISNUMBER(C152),"arith_" &amp; INDEX(Operations[],J152,2) &amp; "_g" &amp; TEXT(C152, "00") &amp; "_" &amp; TEXT(D152, "00") &amp; "_o" &amp; TEXT(E152, "00") &amp; IF(AND(ISNUMBER(F152), F152&lt;&gt;E152), "_" &amp; TEXT(F152, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C152),"arith_" &amp; INDEX(Operations[],J152,2) &amp; "_g" &amp; TEXT(C152, "00") &amp; "_" &amp; TEXT(D152, "00") &amp; "_o" &amp; TEXT(E152, "00") &amp; IF(AND(ISNUMBER(F152), F152&gt;E152), "_" &amp; TEXT(F152, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o07_08</v>
       </c>
       <c r="B152" t="str">
@@ -6786,7 +6796,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="str">
-        <f>IF(ISNUMBER(C153),"arith_" &amp; INDEX(Operations[],J153,2) &amp; "_g" &amp; TEXT(C153, "00") &amp; "_" &amp; TEXT(D153, "00") &amp; "_o" &amp; TEXT(E153, "00") &amp; IF(AND(ISNUMBER(F153), F153&lt;&gt;E153), "_" &amp; TEXT(F153, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C153),"arith_" &amp; INDEX(Operations[],J153,2) &amp; "_g" &amp; TEXT(C153, "00") &amp; "_" &amp; TEXT(D153, "00") &amp; "_o" &amp; TEXT(E153, "00") &amp; IF(AND(ISNUMBER(F153), F153&gt;E153), "_" &amp; TEXT(F153, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o08_09</v>
       </c>
       <c r="B153" t="str">
@@ -6828,7 +6838,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="str">
-        <f>IF(ISNUMBER(C154),"arith_" &amp; INDEX(Operations[],J154,2) &amp; "_g" &amp; TEXT(C154, "00") &amp; "_" &amp; TEXT(D154, "00") &amp; "_o" &amp; TEXT(E154, "00") &amp; IF(AND(ISNUMBER(F154), F154&lt;&gt;E154), "_" &amp; TEXT(F154, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C154),"arith_" &amp; INDEX(Operations[],J154,2) &amp; "_g" &amp; TEXT(C154, "00") &amp; "_" &amp; TEXT(D154, "00") &amp; "_o" &amp; TEXT(E154, "00") &amp; IF(AND(ISNUMBER(F154), F154&gt;E154), "_" &amp; TEXT(F154, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o09_10</v>
       </c>
       <c r="B154" t="str">
@@ -6870,7 +6880,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="str">
-        <f>IF(ISNUMBER(C155),"arith_" &amp; INDEX(Operations[],J155,2) &amp; "_g" &amp; TEXT(C155, "00") &amp; "_" &amp; TEXT(D155, "00") &amp; "_o" &amp; TEXT(E155, "00") &amp; IF(AND(ISNUMBER(F155), F155&lt;&gt;E155), "_" &amp; TEXT(F155, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C155),"arith_" &amp; INDEX(Operations[],J155,2) &amp; "_g" &amp; TEXT(C155, "00") &amp; "_" &amp; TEXT(D155, "00") &amp; "_o" &amp; TEXT(E155, "00") &amp; IF(AND(ISNUMBER(F155), F155&gt;E155), "_" &amp; TEXT(F155, "00"), ""), "")</f>
         <v>arith_sub_g04_00_o10</v>
       </c>
       <c r="B155" t="str">
@@ -6912,7 +6922,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="str">
-        <f>IF(ISNUMBER(C156),"arith_" &amp; INDEX(Operations[],J156,2) &amp; "_g" &amp; TEXT(C156, "00") &amp; "_" &amp; TEXT(D156, "00") &amp; "_o" &amp; TEXT(E156, "00") &amp; IF(AND(ISNUMBER(F156), F156&lt;&gt;E156), "_" &amp; TEXT(F156, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C156),"arith_" &amp; INDEX(Operations[],J156,2) &amp; "_g" &amp; TEXT(C156, "00") &amp; "_" &amp; TEXT(D156, "00") &amp; "_o" &amp; TEXT(E156, "00") &amp; IF(AND(ISNUMBER(F156), F156&gt;E156), "_" &amp; TEXT(F156, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B156" t="str">
@@ -6954,7 +6964,7 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="str">
-        <f>IF(ISNUMBER(C157),"arith_" &amp; INDEX(Operations[],J157,2) &amp; "_g" &amp; TEXT(C157, "00") &amp; "_" &amp; TEXT(D157, "00") &amp; "_o" &amp; TEXT(E157, "00") &amp; IF(AND(ISNUMBER(F157), F157&lt;&gt;E157), "_" &amp; TEXT(F157, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C157),"arith_" &amp; INDEX(Operations[],J157,2) &amp; "_g" &amp; TEXT(C157, "00") &amp; "_" &amp; TEXT(D157, "00") &amp; "_o" &amp; TEXT(E157, "00") &amp; IF(AND(ISNUMBER(F157), F157&gt;E157), "_" &amp; TEXT(F157, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o01_02</v>
       </c>
       <c r="B157" t="str">
@@ -6996,7 +7006,7 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="str">
-        <f>IF(ISNUMBER(C158),"arith_" &amp; INDEX(Operations[],J158,2) &amp; "_g" &amp; TEXT(C158, "00") &amp; "_" &amp; TEXT(D158, "00") &amp; "_o" &amp; TEXT(E158, "00") &amp; IF(AND(ISNUMBER(F158), F158&lt;&gt;E158), "_" &amp; TEXT(F158, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C158),"arith_" &amp; INDEX(Operations[],J158,2) &amp; "_g" &amp; TEXT(C158, "00") &amp; "_" &amp; TEXT(D158, "00") &amp; "_o" &amp; TEXT(E158, "00") &amp; IF(AND(ISNUMBER(F158), F158&gt;E158), "_" &amp; TEXT(F158, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o02_03</v>
       </c>
       <c r="B158" t="str">
@@ -7038,7 +7048,7 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="str">
-        <f>IF(ISNUMBER(C159),"arith_" &amp; INDEX(Operations[],J159,2) &amp; "_g" &amp; TEXT(C159, "00") &amp; "_" &amp; TEXT(D159, "00") &amp; "_o" &amp; TEXT(E159, "00") &amp; IF(AND(ISNUMBER(F159), F159&lt;&gt;E159), "_" &amp; TEXT(F159, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C159),"arith_" &amp; INDEX(Operations[],J159,2) &amp; "_g" &amp; TEXT(C159, "00") &amp; "_" &amp; TEXT(D159, "00") &amp; "_o" &amp; TEXT(E159, "00") &amp; IF(AND(ISNUMBER(F159), F159&gt;E159), "_" &amp; TEXT(F159, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o03_04</v>
       </c>
       <c r="B159" t="str">
@@ -7080,7 +7090,7 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="str">
-        <f>IF(ISNUMBER(C160),"arith_" &amp; INDEX(Operations[],J160,2) &amp; "_g" &amp; TEXT(C160, "00") &amp; "_" &amp; TEXT(D160, "00") &amp; "_o" &amp; TEXT(E160, "00") &amp; IF(AND(ISNUMBER(F160), F160&lt;&gt;E160), "_" &amp; TEXT(F160, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C160),"arith_" &amp; INDEX(Operations[],J160,2) &amp; "_g" &amp; TEXT(C160, "00") &amp; "_" &amp; TEXT(D160, "00") &amp; "_o" &amp; TEXT(E160, "00") &amp; IF(AND(ISNUMBER(F160), F160&gt;E160), "_" &amp; TEXT(F160, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o04_05</v>
       </c>
       <c r="B160" t="str">
@@ -7122,7 +7132,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="str">
-        <f>IF(ISNUMBER(C161),"arith_" &amp; INDEX(Operations[],J161,2) &amp; "_g" &amp; TEXT(C161, "00") &amp; "_" &amp; TEXT(D161, "00") &amp; "_o" &amp; TEXT(E161, "00") &amp; IF(AND(ISNUMBER(F161), F161&lt;&gt;E161), "_" &amp; TEXT(F161, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C161),"arith_" &amp; INDEX(Operations[],J161,2) &amp; "_g" &amp; TEXT(C161, "00") &amp; "_" &amp; TEXT(D161, "00") &amp; "_o" &amp; TEXT(E161, "00") &amp; IF(AND(ISNUMBER(F161), F161&gt;E161), "_" &amp; TEXT(F161, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o05_06</v>
       </c>
       <c r="B161" t="str">
@@ -7164,7 +7174,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="str">
-        <f>IF(ISNUMBER(C162),"arith_" &amp; INDEX(Operations[],J162,2) &amp; "_g" &amp; TEXT(C162, "00") &amp; "_" &amp; TEXT(D162, "00") &amp; "_o" &amp; TEXT(E162, "00") &amp; IF(AND(ISNUMBER(F162), F162&lt;&gt;E162), "_" &amp; TEXT(F162, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C162),"arith_" &amp; INDEX(Operations[],J162,2) &amp; "_g" &amp; TEXT(C162, "00") &amp; "_" &amp; TEXT(D162, "00") &amp; "_o" &amp; TEXT(E162, "00") &amp; IF(AND(ISNUMBER(F162), F162&gt;E162), "_" &amp; TEXT(F162, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o06_07</v>
       </c>
       <c r="B162" t="str">
@@ -7206,7 +7216,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="str">
-        <f>IF(ISNUMBER(C163),"arith_" &amp; INDEX(Operations[],J163,2) &amp; "_g" &amp; TEXT(C163, "00") &amp; "_" &amp; TEXT(D163, "00") &amp; "_o" &amp; TEXT(E163, "00") &amp; IF(AND(ISNUMBER(F163), F163&lt;&gt;E163), "_" &amp; TEXT(F163, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C163),"arith_" &amp; INDEX(Operations[],J163,2) &amp; "_g" &amp; TEXT(C163, "00") &amp; "_" &amp; TEXT(D163, "00") &amp; "_o" &amp; TEXT(E163, "00") &amp; IF(AND(ISNUMBER(F163), F163&gt;E163), "_" &amp; TEXT(F163, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o07_08</v>
       </c>
       <c r="B163" t="str">
@@ -7248,7 +7258,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="str">
-        <f>IF(ISNUMBER(C164),"arith_" &amp; INDEX(Operations[],J164,2) &amp; "_g" &amp; TEXT(C164, "00") &amp; "_" &amp; TEXT(D164, "00") &amp; "_o" &amp; TEXT(E164, "00") &amp; IF(AND(ISNUMBER(F164), F164&lt;&gt;E164), "_" &amp; TEXT(F164, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C164),"arith_" &amp; INDEX(Operations[],J164,2) &amp; "_g" &amp; TEXT(C164, "00") &amp; "_" &amp; TEXT(D164, "00") &amp; "_o" &amp; TEXT(E164, "00") &amp; IF(AND(ISNUMBER(F164), F164&gt;E164), "_" &amp; TEXT(F164, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o08_09</v>
       </c>
       <c r="B164" t="str">
@@ -7290,7 +7300,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="str">
-        <f>IF(ISNUMBER(C165),"arith_" &amp; INDEX(Operations[],J165,2) &amp; "_g" &amp; TEXT(C165, "00") &amp; "_" &amp; TEXT(D165, "00") &amp; "_o" &amp; TEXT(E165, "00") &amp; IF(AND(ISNUMBER(F165), F165&lt;&gt;E165), "_" &amp; TEXT(F165, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C165),"arith_" &amp; INDEX(Operations[],J165,2) &amp; "_g" &amp; TEXT(C165, "00") &amp; "_" &amp; TEXT(D165, "00") &amp; "_o" &amp; TEXT(E165, "00") &amp; IF(AND(ISNUMBER(F165), F165&gt;E165), "_" &amp; TEXT(F165, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o09_10</v>
       </c>
       <c r="B165" t="str">
@@ -7332,7 +7342,7 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="str">
-        <f>IF(ISNUMBER(C166),"arith_" &amp; INDEX(Operations[],J166,2) &amp; "_g" &amp; TEXT(C166, "00") &amp; "_" &amp; TEXT(D166, "00") &amp; "_o" &amp; TEXT(E166, "00") &amp; IF(AND(ISNUMBER(F166), F166&lt;&gt;E166), "_" &amp; TEXT(F166, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C166),"arith_" &amp; INDEX(Operations[],J166,2) &amp; "_g" &amp; TEXT(C166, "00") &amp; "_" &amp; TEXT(D166, "00") &amp; "_o" &amp; TEXT(E166, "00") &amp; IF(AND(ISNUMBER(F166), F166&gt;E166), "_" &amp; TEXT(F166, "00"), ""), "")</f>
         <v>arith_sub_g05_00_o10</v>
       </c>
       <c r="B166" t="str">
@@ -7374,7 +7384,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="str">
-        <f>IF(ISNUMBER(C167),"arith_" &amp; INDEX(Operations[],J167,2) &amp; "_g" &amp; TEXT(C167, "00") &amp; "_" &amp; TEXT(D167, "00") &amp; "_o" &amp; TEXT(E167, "00") &amp; IF(AND(ISNUMBER(F167), F167&lt;&gt;E167), "_" &amp; TEXT(F167, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C167),"arith_" &amp; INDEX(Operations[],J167,2) &amp; "_g" &amp; TEXT(C167, "00") &amp; "_" &amp; TEXT(D167, "00") &amp; "_o" &amp; TEXT(E167, "00") &amp; IF(AND(ISNUMBER(F167), F167&gt;E167), "_" &amp; TEXT(F167, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B167" t="str">
@@ -7416,7 +7426,7 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="str">
-        <f>IF(ISNUMBER(C168),"arith_" &amp; INDEX(Operations[],J168,2) &amp; "_g" &amp; TEXT(C168, "00") &amp; "_" &amp; TEXT(D168, "00") &amp; "_o" &amp; TEXT(E168, "00") &amp; IF(AND(ISNUMBER(F168), F168&lt;&gt;E168), "_" &amp; TEXT(F168, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C168),"arith_" &amp; INDEX(Operations[],J168,2) &amp; "_g" &amp; TEXT(C168, "00") &amp; "_" &amp; TEXT(D168, "00") &amp; "_o" &amp; TEXT(E168, "00") &amp; IF(AND(ISNUMBER(F168), F168&gt;E168), "_" &amp; TEXT(F168, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o01_02</v>
       </c>
       <c r="B168" t="str">
@@ -7458,7 +7468,7 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="str">
-        <f>IF(ISNUMBER(C169),"arith_" &amp; INDEX(Operations[],J169,2) &amp; "_g" &amp; TEXT(C169, "00") &amp; "_" &amp; TEXT(D169, "00") &amp; "_o" &amp; TEXT(E169, "00") &amp; IF(AND(ISNUMBER(F169), F169&lt;&gt;E169), "_" &amp; TEXT(F169, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C169),"arith_" &amp; INDEX(Operations[],J169,2) &amp; "_g" &amp; TEXT(C169, "00") &amp; "_" &amp; TEXT(D169, "00") &amp; "_o" &amp; TEXT(E169, "00") &amp; IF(AND(ISNUMBER(F169), F169&gt;E169), "_" &amp; TEXT(F169, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o02_03</v>
       </c>
       <c r="B169" t="str">
@@ -7500,7 +7510,7 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="str">
-        <f>IF(ISNUMBER(C170),"arith_" &amp; INDEX(Operations[],J170,2) &amp; "_g" &amp; TEXT(C170, "00") &amp; "_" &amp; TEXT(D170, "00") &amp; "_o" &amp; TEXT(E170, "00") &amp; IF(AND(ISNUMBER(F170), F170&lt;&gt;E170), "_" &amp; TEXT(F170, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C170),"arith_" &amp; INDEX(Operations[],J170,2) &amp; "_g" &amp; TEXT(C170, "00") &amp; "_" &amp; TEXT(D170, "00") &amp; "_o" &amp; TEXT(E170, "00") &amp; IF(AND(ISNUMBER(F170), F170&gt;E170), "_" &amp; TEXT(F170, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o03_04</v>
       </c>
       <c r="B170" t="str">
@@ -7542,7 +7552,7 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
-        <f>IF(ISNUMBER(C171),"arith_" &amp; INDEX(Operations[],J171,2) &amp; "_g" &amp; TEXT(C171, "00") &amp; "_" &amp; TEXT(D171, "00") &amp; "_o" &amp; TEXT(E171, "00") &amp; IF(AND(ISNUMBER(F171), F171&lt;&gt;E171), "_" &amp; TEXT(F171, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C171),"arith_" &amp; INDEX(Operations[],J171,2) &amp; "_g" &amp; TEXT(C171, "00") &amp; "_" &amp; TEXT(D171, "00") &amp; "_o" &amp; TEXT(E171, "00") &amp; IF(AND(ISNUMBER(F171), F171&gt;E171), "_" &amp; TEXT(F171, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o04_05</v>
       </c>
       <c r="B171" t="str">
@@ -7584,7 +7594,7 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="str">
-        <f>IF(ISNUMBER(C172),"arith_" &amp; INDEX(Operations[],J172,2) &amp; "_g" &amp; TEXT(C172, "00") &amp; "_" &amp; TEXT(D172, "00") &amp; "_o" &amp; TEXT(E172, "00") &amp; IF(AND(ISNUMBER(F172), F172&lt;&gt;E172), "_" &amp; TEXT(F172, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C172),"arith_" &amp; INDEX(Operations[],J172,2) &amp; "_g" &amp; TEXT(C172, "00") &amp; "_" &amp; TEXT(D172, "00") &amp; "_o" &amp; TEXT(E172, "00") &amp; IF(AND(ISNUMBER(F172), F172&gt;E172), "_" &amp; TEXT(F172, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o05_06</v>
       </c>
       <c r="B172" t="str">
@@ -7626,7 +7636,7 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="str">
-        <f>IF(ISNUMBER(C173),"arith_" &amp; INDEX(Operations[],J173,2) &amp; "_g" &amp; TEXT(C173, "00") &amp; "_" &amp; TEXT(D173, "00") &amp; "_o" &amp; TEXT(E173, "00") &amp; IF(AND(ISNUMBER(F173), F173&lt;&gt;E173), "_" &amp; TEXT(F173, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C173),"arith_" &amp; INDEX(Operations[],J173,2) &amp; "_g" &amp; TEXT(C173, "00") &amp; "_" &amp; TEXT(D173, "00") &amp; "_o" &amp; TEXT(E173, "00") &amp; IF(AND(ISNUMBER(F173), F173&gt;E173), "_" &amp; TEXT(F173, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o06_07</v>
       </c>
       <c r="B173" t="str">
@@ -7668,7 +7678,7 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
-        <f>IF(ISNUMBER(C174),"arith_" &amp; INDEX(Operations[],J174,2) &amp; "_g" &amp; TEXT(C174, "00") &amp; "_" &amp; TEXT(D174, "00") &amp; "_o" &amp; TEXT(E174, "00") &amp; IF(AND(ISNUMBER(F174), F174&lt;&gt;E174), "_" &amp; TEXT(F174, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C174),"arith_" &amp; INDEX(Operations[],J174,2) &amp; "_g" &amp; TEXT(C174, "00") &amp; "_" &amp; TEXT(D174, "00") &amp; "_o" &amp; TEXT(E174, "00") &amp; IF(AND(ISNUMBER(F174), F174&gt;E174), "_" &amp; TEXT(F174, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o07_08</v>
       </c>
       <c r="B174" t="str">
@@ -7710,7 +7720,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="str">
-        <f>IF(ISNUMBER(C175),"arith_" &amp; INDEX(Operations[],J175,2) &amp; "_g" &amp; TEXT(C175, "00") &amp; "_" &amp; TEXT(D175, "00") &amp; "_o" &amp; TEXT(E175, "00") &amp; IF(AND(ISNUMBER(F175), F175&lt;&gt;E175), "_" &amp; TEXT(F175, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C175),"arith_" &amp; INDEX(Operations[],J175,2) &amp; "_g" &amp; TEXT(C175, "00") &amp; "_" &amp; TEXT(D175, "00") &amp; "_o" &amp; TEXT(E175, "00") &amp; IF(AND(ISNUMBER(F175), F175&gt;E175), "_" &amp; TEXT(F175, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o08_09</v>
       </c>
       <c r="B175" t="str">
@@ -7752,7 +7762,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="str">
-        <f>IF(ISNUMBER(C176),"arith_" &amp; INDEX(Operations[],J176,2) &amp; "_g" &amp; TEXT(C176, "00") &amp; "_" &amp; TEXT(D176, "00") &amp; "_o" &amp; TEXT(E176, "00") &amp; IF(AND(ISNUMBER(F176), F176&lt;&gt;E176), "_" &amp; TEXT(F176, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C176),"arith_" &amp; INDEX(Operations[],J176,2) &amp; "_g" &amp; TEXT(C176, "00") &amp; "_" &amp; TEXT(D176, "00") &amp; "_o" &amp; TEXT(E176, "00") &amp; IF(AND(ISNUMBER(F176), F176&gt;E176), "_" &amp; TEXT(F176, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o09_10</v>
       </c>
       <c r="B176" t="str">
@@ -7794,7 +7804,7 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
-        <f>IF(ISNUMBER(C177),"arith_" &amp; INDEX(Operations[],J177,2) &amp; "_g" &amp; TEXT(C177, "00") &amp; "_" &amp; TEXT(D177, "00") &amp; "_o" &amp; TEXT(E177, "00") &amp; IF(AND(ISNUMBER(F177), F177&lt;&gt;E177), "_" &amp; TEXT(F177, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C177),"arith_" &amp; INDEX(Operations[],J177,2) &amp; "_g" &amp; TEXT(C177, "00") &amp; "_" &amp; TEXT(D177, "00") &amp; "_o" &amp; TEXT(E177, "00") &amp; IF(AND(ISNUMBER(F177), F177&gt;E177), "_" &amp; TEXT(F177, "00"), ""), "")</f>
         <v>arith_sub_g06_00_o10</v>
       </c>
       <c r="B177" t="str">
@@ -7836,7 +7846,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="str">
-        <f>IF(ISNUMBER(C178),"arith_" &amp; INDEX(Operations[],J178,2) &amp; "_g" &amp; TEXT(C178, "00") &amp; "_" &amp; TEXT(D178, "00") &amp; "_o" &amp; TEXT(E178, "00") &amp; IF(AND(ISNUMBER(F178), F178&lt;&gt;E178), "_" &amp; TEXT(F178, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C178),"arith_" &amp; INDEX(Operations[],J178,2) &amp; "_g" &amp; TEXT(C178, "00") &amp; "_" &amp; TEXT(D178, "00") &amp; "_o" &amp; TEXT(E178, "00") &amp; IF(AND(ISNUMBER(F178), F178&gt;E178), "_" &amp; TEXT(F178, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B178" t="str">
@@ -7878,7 +7888,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="str">
-        <f>IF(ISNUMBER(C179),"arith_" &amp; INDEX(Operations[],J179,2) &amp; "_g" &amp; TEXT(C179, "00") &amp; "_" &amp; TEXT(D179, "00") &amp; "_o" &amp; TEXT(E179, "00") &amp; IF(AND(ISNUMBER(F179), F179&lt;&gt;E179), "_" &amp; TEXT(F179, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C179),"arith_" &amp; INDEX(Operations[],J179,2) &amp; "_g" &amp; TEXT(C179, "00") &amp; "_" &amp; TEXT(D179, "00") &amp; "_o" &amp; TEXT(E179, "00") &amp; IF(AND(ISNUMBER(F179), F179&gt;E179), "_" &amp; TEXT(F179, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o01_02</v>
       </c>
       <c r="B179" t="str">
@@ -7920,7 +7930,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="str">
-        <f>IF(ISNUMBER(C180),"arith_" &amp; INDEX(Operations[],J180,2) &amp; "_g" &amp; TEXT(C180, "00") &amp; "_" &amp; TEXT(D180, "00") &amp; "_o" &amp; TEXT(E180, "00") &amp; IF(AND(ISNUMBER(F180), F180&lt;&gt;E180), "_" &amp; TEXT(F180, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C180),"arith_" &amp; INDEX(Operations[],J180,2) &amp; "_g" &amp; TEXT(C180, "00") &amp; "_" &amp; TEXT(D180, "00") &amp; "_o" &amp; TEXT(E180, "00") &amp; IF(AND(ISNUMBER(F180), F180&gt;E180), "_" &amp; TEXT(F180, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o02_03</v>
       </c>
       <c r="B180" t="str">
@@ -7962,7 +7972,7 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="str">
-        <f>IF(ISNUMBER(C181),"arith_" &amp; INDEX(Operations[],J181,2) &amp; "_g" &amp; TEXT(C181, "00") &amp; "_" &amp; TEXT(D181, "00") &amp; "_o" &amp; TEXT(E181, "00") &amp; IF(AND(ISNUMBER(F181), F181&lt;&gt;E181), "_" &amp; TEXT(F181, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C181),"arith_" &amp; INDEX(Operations[],J181,2) &amp; "_g" &amp; TEXT(C181, "00") &amp; "_" &amp; TEXT(D181, "00") &amp; "_o" &amp; TEXT(E181, "00") &amp; IF(AND(ISNUMBER(F181), F181&gt;E181), "_" &amp; TEXT(F181, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o03_04</v>
       </c>
       <c r="B181" t="str">
@@ -8004,7 +8014,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="str">
-        <f>IF(ISNUMBER(C182),"arith_" &amp; INDEX(Operations[],J182,2) &amp; "_g" &amp; TEXT(C182, "00") &amp; "_" &amp; TEXT(D182, "00") &amp; "_o" &amp; TEXT(E182, "00") &amp; IF(AND(ISNUMBER(F182), F182&lt;&gt;E182), "_" &amp; TEXT(F182, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C182),"arith_" &amp; INDEX(Operations[],J182,2) &amp; "_g" &amp; TEXT(C182, "00") &amp; "_" &amp; TEXT(D182, "00") &amp; "_o" &amp; TEXT(E182, "00") &amp; IF(AND(ISNUMBER(F182), F182&gt;E182), "_" &amp; TEXT(F182, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o04_05</v>
       </c>
       <c r="B182" t="str">
@@ -8046,7 +8056,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="str">
-        <f>IF(ISNUMBER(C183),"arith_" &amp; INDEX(Operations[],J183,2) &amp; "_g" &amp; TEXT(C183, "00") &amp; "_" &amp; TEXT(D183, "00") &amp; "_o" &amp; TEXT(E183, "00") &amp; IF(AND(ISNUMBER(F183), F183&lt;&gt;E183), "_" &amp; TEXT(F183, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C183),"arith_" &amp; INDEX(Operations[],J183,2) &amp; "_g" &amp; TEXT(C183, "00") &amp; "_" &amp; TEXT(D183, "00") &amp; "_o" &amp; TEXT(E183, "00") &amp; IF(AND(ISNUMBER(F183), F183&gt;E183), "_" &amp; TEXT(F183, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o05_06</v>
       </c>
       <c r="B183" t="str">
@@ -8088,7 +8098,7 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="str">
-        <f>IF(ISNUMBER(C184),"arith_" &amp; INDEX(Operations[],J184,2) &amp; "_g" &amp; TEXT(C184, "00") &amp; "_" &amp; TEXT(D184, "00") &amp; "_o" &amp; TEXT(E184, "00") &amp; IF(AND(ISNUMBER(F184), F184&lt;&gt;E184), "_" &amp; TEXT(F184, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C184),"arith_" &amp; INDEX(Operations[],J184,2) &amp; "_g" &amp; TEXT(C184, "00") &amp; "_" &amp; TEXT(D184, "00") &amp; "_o" &amp; TEXT(E184, "00") &amp; IF(AND(ISNUMBER(F184), F184&gt;E184), "_" &amp; TEXT(F184, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o06_07</v>
       </c>
       <c r="B184" t="str">
@@ -8130,7 +8140,7 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="str">
-        <f>IF(ISNUMBER(C185),"arith_" &amp; INDEX(Operations[],J185,2) &amp; "_g" &amp; TEXT(C185, "00") &amp; "_" &amp; TEXT(D185, "00") &amp; "_o" &amp; TEXT(E185, "00") &amp; IF(AND(ISNUMBER(F185), F185&lt;&gt;E185), "_" &amp; TEXT(F185, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C185),"arith_" &amp; INDEX(Operations[],J185,2) &amp; "_g" &amp; TEXT(C185, "00") &amp; "_" &amp; TEXT(D185, "00") &amp; "_o" &amp; TEXT(E185, "00") &amp; IF(AND(ISNUMBER(F185), F185&gt;E185), "_" &amp; TEXT(F185, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o07_08</v>
       </c>
       <c r="B185" t="str">
@@ -8172,7 +8182,7 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="str">
-        <f>IF(ISNUMBER(C186),"arith_" &amp; INDEX(Operations[],J186,2) &amp; "_g" &amp; TEXT(C186, "00") &amp; "_" &amp; TEXT(D186, "00") &amp; "_o" &amp; TEXT(E186, "00") &amp; IF(AND(ISNUMBER(F186), F186&lt;&gt;E186), "_" &amp; TEXT(F186, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C186),"arith_" &amp; INDEX(Operations[],J186,2) &amp; "_g" &amp; TEXT(C186, "00") &amp; "_" &amp; TEXT(D186, "00") &amp; "_o" &amp; TEXT(E186, "00") &amp; IF(AND(ISNUMBER(F186), F186&gt;E186), "_" &amp; TEXT(F186, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o08_09</v>
       </c>
       <c r="B186" t="str">
@@ -8214,7 +8224,7 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="str">
-        <f>IF(ISNUMBER(C187),"arith_" &amp; INDEX(Operations[],J187,2) &amp; "_g" &amp; TEXT(C187, "00") &amp; "_" &amp; TEXT(D187, "00") &amp; "_o" &amp; TEXT(E187, "00") &amp; IF(AND(ISNUMBER(F187), F187&lt;&gt;E187), "_" &amp; TEXT(F187, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C187),"arith_" &amp; INDEX(Operations[],J187,2) &amp; "_g" &amp; TEXT(C187, "00") &amp; "_" &amp; TEXT(D187, "00") &amp; "_o" &amp; TEXT(E187, "00") &amp; IF(AND(ISNUMBER(F187), F187&gt;E187), "_" &amp; TEXT(F187, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o09_10</v>
       </c>
       <c r="B187" t="str">
@@ -8256,7 +8266,7 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="str">
-        <f>IF(ISNUMBER(C188),"arith_" &amp; INDEX(Operations[],J188,2) &amp; "_g" &amp; TEXT(C188, "00") &amp; "_" &amp; TEXT(D188, "00") &amp; "_o" &amp; TEXT(E188, "00") &amp; IF(AND(ISNUMBER(F188), F188&lt;&gt;E188), "_" &amp; TEXT(F188, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C188),"arith_" &amp; INDEX(Operations[],J188,2) &amp; "_g" &amp; TEXT(C188, "00") &amp; "_" &amp; TEXT(D188, "00") &amp; "_o" &amp; TEXT(E188, "00") &amp; IF(AND(ISNUMBER(F188), F188&gt;E188), "_" &amp; TEXT(F188, "00"), ""), "")</f>
         <v>arith_sub_g07_00_o10</v>
       </c>
       <c r="B188" t="str">
@@ -8298,7 +8308,7 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="str">
-        <f>IF(ISNUMBER(C189),"arith_" &amp; INDEX(Operations[],J189,2) &amp; "_g" &amp; TEXT(C189, "00") &amp; "_" &amp; TEXT(D189, "00") &amp; "_o" &amp; TEXT(E189, "00") &amp; IF(AND(ISNUMBER(F189), F189&lt;&gt;E189), "_" &amp; TEXT(F189, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C189),"arith_" &amp; INDEX(Operations[],J189,2) &amp; "_g" &amp; TEXT(C189, "00") &amp; "_" &amp; TEXT(D189, "00") &amp; "_o" &amp; TEXT(E189, "00") &amp; IF(AND(ISNUMBER(F189), F189&gt;E189), "_" &amp; TEXT(F189, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B189" t="str">
@@ -8340,7 +8350,7 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="str">
-        <f>IF(ISNUMBER(C190),"arith_" &amp; INDEX(Operations[],J190,2) &amp; "_g" &amp; TEXT(C190, "00") &amp; "_" &amp; TEXT(D190, "00") &amp; "_o" &amp; TEXT(E190, "00") &amp; IF(AND(ISNUMBER(F190), F190&lt;&gt;E190), "_" &amp; TEXT(F190, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C190),"arith_" &amp; INDEX(Operations[],J190,2) &amp; "_g" &amp; TEXT(C190, "00") &amp; "_" &amp; TEXT(D190, "00") &amp; "_o" &amp; TEXT(E190, "00") &amp; IF(AND(ISNUMBER(F190), F190&gt;E190), "_" &amp; TEXT(F190, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o01_02</v>
       </c>
       <c r="B190" t="str">
@@ -8382,7 +8392,7 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="str">
-        <f>IF(ISNUMBER(C191),"arith_" &amp; INDEX(Operations[],J191,2) &amp; "_g" &amp; TEXT(C191, "00") &amp; "_" &amp; TEXT(D191, "00") &amp; "_o" &amp; TEXT(E191, "00") &amp; IF(AND(ISNUMBER(F191), F191&lt;&gt;E191), "_" &amp; TEXT(F191, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C191),"arith_" &amp; INDEX(Operations[],J191,2) &amp; "_g" &amp; TEXT(C191, "00") &amp; "_" &amp; TEXT(D191, "00") &amp; "_o" &amp; TEXT(E191, "00") &amp; IF(AND(ISNUMBER(F191), F191&gt;E191), "_" &amp; TEXT(F191, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o02_03</v>
       </c>
       <c r="B191" t="str">
@@ -8424,7 +8434,7 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="str">
-        <f>IF(ISNUMBER(C192),"arith_" &amp; INDEX(Operations[],J192,2) &amp; "_g" &amp; TEXT(C192, "00") &amp; "_" &amp; TEXT(D192, "00") &amp; "_o" &amp; TEXT(E192, "00") &amp; IF(AND(ISNUMBER(F192), F192&lt;&gt;E192), "_" &amp; TEXT(F192, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C192),"arith_" &amp; INDEX(Operations[],J192,2) &amp; "_g" &amp; TEXT(C192, "00") &amp; "_" &amp; TEXT(D192, "00") &amp; "_o" &amp; TEXT(E192, "00") &amp; IF(AND(ISNUMBER(F192), F192&gt;E192), "_" &amp; TEXT(F192, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o03_04</v>
       </c>
       <c r="B192" t="str">
@@ -8466,7 +8476,7 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="str">
-        <f>IF(ISNUMBER(C193),"arith_" &amp; INDEX(Operations[],J193,2) &amp; "_g" &amp; TEXT(C193, "00") &amp; "_" &amp; TEXT(D193, "00") &amp; "_o" &amp; TEXT(E193, "00") &amp; IF(AND(ISNUMBER(F193), F193&lt;&gt;E193), "_" &amp; TEXT(F193, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C193),"arith_" &amp; INDEX(Operations[],J193,2) &amp; "_g" &amp; TEXT(C193, "00") &amp; "_" &amp; TEXT(D193, "00") &amp; "_o" &amp; TEXT(E193, "00") &amp; IF(AND(ISNUMBER(F193), F193&gt;E193), "_" &amp; TEXT(F193, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o04_05</v>
       </c>
       <c r="B193" t="str">
@@ -8508,7 +8518,7 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="str">
-        <f>IF(ISNUMBER(C194),"arith_" &amp; INDEX(Operations[],J194,2) &amp; "_g" &amp; TEXT(C194, "00") &amp; "_" &amp; TEXT(D194, "00") &amp; "_o" &amp; TEXT(E194, "00") &amp; IF(AND(ISNUMBER(F194), F194&lt;&gt;E194), "_" &amp; TEXT(F194, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C194),"arith_" &amp; INDEX(Operations[],J194,2) &amp; "_g" &amp; TEXT(C194, "00") &amp; "_" &amp; TEXT(D194, "00") &amp; "_o" &amp; TEXT(E194, "00") &amp; IF(AND(ISNUMBER(F194), F194&gt;E194), "_" &amp; TEXT(F194, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o05_06</v>
       </c>
       <c r="B194" t="str">
@@ -8550,7 +8560,7 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="str">
-        <f>IF(ISNUMBER(C195),"arith_" &amp; INDEX(Operations[],J195,2) &amp; "_g" &amp; TEXT(C195, "00") &amp; "_" &amp; TEXT(D195, "00") &amp; "_o" &amp; TEXT(E195, "00") &amp; IF(AND(ISNUMBER(F195), F195&lt;&gt;E195), "_" &amp; TEXT(F195, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C195),"arith_" &amp; INDEX(Operations[],J195,2) &amp; "_g" &amp; TEXT(C195, "00") &amp; "_" &amp; TEXT(D195, "00") &amp; "_o" &amp; TEXT(E195, "00") &amp; IF(AND(ISNUMBER(F195), F195&gt;E195), "_" &amp; TEXT(F195, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o06_07</v>
       </c>
       <c r="B195" t="str">
@@ -8592,7 +8602,7 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="str">
-        <f>IF(ISNUMBER(C196),"arith_" &amp; INDEX(Operations[],J196,2) &amp; "_g" &amp; TEXT(C196, "00") &amp; "_" &amp; TEXT(D196, "00") &amp; "_o" &amp; TEXT(E196, "00") &amp; IF(AND(ISNUMBER(F196), F196&lt;&gt;E196), "_" &amp; TEXT(F196, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C196),"arith_" &amp; INDEX(Operations[],J196,2) &amp; "_g" &amp; TEXT(C196, "00") &amp; "_" &amp; TEXT(D196, "00") &amp; "_o" &amp; TEXT(E196, "00") &amp; IF(AND(ISNUMBER(F196), F196&gt;E196), "_" &amp; TEXT(F196, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o07_08</v>
       </c>
       <c r="B196" t="str">
@@ -8634,7 +8644,7 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="str">
-        <f>IF(ISNUMBER(C197),"arith_" &amp; INDEX(Operations[],J197,2) &amp; "_g" &amp; TEXT(C197, "00") &amp; "_" &amp; TEXT(D197, "00") &amp; "_o" &amp; TEXT(E197, "00") &amp; IF(AND(ISNUMBER(F197), F197&lt;&gt;E197), "_" &amp; TEXT(F197, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C197),"arith_" &amp; INDEX(Operations[],J197,2) &amp; "_g" &amp; TEXT(C197, "00") &amp; "_" &amp; TEXT(D197, "00") &amp; "_o" &amp; TEXT(E197, "00") &amp; IF(AND(ISNUMBER(F197), F197&gt;E197), "_" &amp; TEXT(F197, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o08_09</v>
       </c>
       <c r="B197" t="str">
@@ -8676,7 +8686,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="str">
-        <f>IF(ISNUMBER(C198),"arith_" &amp; INDEX(Operations[],J198,2) &amp; "_g" &amp; TEXT(C198, "00") &amp; "_" &amp; TEXT(D198, "00") &amp; "_o" &amp; TEXT(E198, "00") &amp; IF(AND(ISNUMBER(F198), F198&lt;&gt;E198), "_" &amp; TEXT(F198, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C198),"arith_" &amp; INDEX(Operations[],J198,2) &amp; "_g" &amp; TEXT(C198, "00") &amp; "_" &amp; TEXT(D198, "00") &amp; "_o" &amp; TEXT(E198, "00") &amp; IF(AND(ISNUMBER(F198), F198&gt;E198), "_" &amp; TEXT(F198, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o09_10</v>
       </c>
       <c r="B198" t="str">
@@ -8718,7 +8728,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="str">
-        <f>IF(ISNUMBER(C199),"arith_" &amp; INDEX(Operations[],J199,2) &amp; "_g" &amp; TEXT(C199, "00") &amp; "_" &amp; TEXT(D199, "00") &amp; "_o" &amp; TEXT(E199, "00") &amp; IF(AND(ISNUMBER(F199), F199&lt;&gt;E199), "_" &amp; TEXT(F199, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C199),"arith_" &amp; INDEX(Operations[],J199,2) &amp; "_g" &amp; TEXT(C199, "00") &amp; "_" &amp; TEXT(D199, "00") &amp; "_o" &amp; TEXT(E199, "00") &amp; IF(AND(ISNUMBER(F199), F199&gt;E199), "_" &amp; TEXT(F199, "00"), ""), "")</f>
         <v>arith_sub_g08_00_o10</v>
       </c>
       <c r="B199" t="str">
@@ -8760,7 +8770,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="str">
-        <f>IF(ISNUMBER(C200),"arith_" &amp; INDEX(Operations[],J200,2) &amp; "_g" &amp; TEXT(C200, "00") &amp; "_" &amp; TEXT(D200, "00") &amp; "_o" &amp; TEXT(E200, "00") &amp; IF(AND(ISNUMBER(F200), F200&lt;&gt;E200), "_" &amp; TEXT(F200, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C200),"arith_" &amp; INDEX(Operations[],J200,2) &amp; "_g" &amp; TEXT(C200, "00") &amp; "_" &amp; TEXT(D200, "00") &amp; "_o" &amp; TEXT(E200, "00") &amp; IF(AND(ISNUMBER(F200), F200&gt;E200), "_" &amp; TEXT(F200, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B200" t="str">
@@ -8802,7 +8812,7 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="str">
-        <f>IF(ISNUMBER(C201),"arith_" &amp; INDEX(Operations[],J201,2) &amp; "_g" &amp; TEXT(C201, "00") &amp; "_" &amp; TEXT(D201, "00") &amp; "_o" &amp; TEXT(E201, "00") &amp; IF(AND(ISNUMBER(F201), F201&lt;&gt;E201), "_" &amp; TEXT(F201, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C201),"arith_" &amp; INDEX(Operations[],J201,2) &amp; "_g" &amp; TEXT(C201, "00") &amp; "_" &amp; TEXT(D201, "00") &amp; "_o" &amp; TEXT(E201, "00") &amp; IF(AND(ISNUMBER(F201), F201&gt;E201), "_" &amp; TEXT(F201, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o01_02</v>
       </c>
       <c r="B201" t="str">
@@ -8844,7 +8854,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="str">
-        <f>IF(ISNUMBER(C202),"arith_" &amp; INDEX(Operations[],J202,2) &amp; "_g" &amp; TEXT(C202, "00") &amp; "_" &amp; TEXT(D202, "00") &amp; "_o" &amp; TEXT(E202, "00") &amp; IF(AND(ISNUMBER(F202), F202&lt;&gt;E202), "_" &amp; TEXT(F202, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C202),"arith_" &amp; INDEX(Operations[],J202,2) &amp; "_g" &amp; TEXT(C202, "00") &amp; "_" &amp; TEXT(D202, "00") &amp; "_o" &amp; TEXT(E202, "00") &amp; IF(AND(ISNUMBER(F202), F202&gt;E202), "_" &amp; TEXT(F202, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o02_03</v>
       </c>
       <c r="B202" t="str">
@@ -8886,7 +8896,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="str">
-        <f>IF(ISNUMBER(C203),"arith_" &amp; INDEX(Operations[],J203,2) &amp; "_g" &amp; TEXT(C203, "00") &amp; "_" &amp; TEXT(D203, "00") &amp; "_o" &amp; TEXT(E203, "00") &amp; IF(AND(ISNUMBER(F203), F203&lt;&gt;E203), "_" &amp; TEXT(F203, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C203),"arith_" &amp; INDEX(Operations[],J203,2) &amp; "_g" &amp; TEXT(C203, "00") &amp; "_" &amp; TEXT(D203, "00") &amp; "_o" &amp; TEXT(E203, "00") &amp; IF(AND(ISNUMBER(F203), F203&gt;E203), "_" &amp; TEXT(F203, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o03_04</v>
       </c>
       <c r="B203" t="str">
@@ -8928,7 +8938,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="str">
-        <f>IF(ISNUMBER(C204),"arith_" &amp; INDEX(Operations[],J204,2) &amp; "_g" &amp; TEXT(C204, "00") &amp; "_" &amp; TEXT(D204, "00") &amp; "_o" &amp; TEXT(E204, "00") &amp; IF(AND(ISNUMBER(F204), F204&lt;&gt;E204), "_" &amp; TEXT(F204, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C204),"arith_" &amp; INDEX(Operations[],J204,2) &amp; "_g" &amp; TEXT(C204, "00") &amp; "_" &amp; TEXT(D204, "00") &amp; "_o" &amp; TEXT(E204, "00") &amp; IF(AND(ISNUMBER(F204), F204&gt;E204), "_" &amp; TEXT(F204, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o04_05</v>
       </c>
       <c r="B204" t="str">
@@ -8970,7 +8980,7 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="str">
-        <f>IF(ISNUMBER(C205),"arith_" &amp; INDEX(Operations[],J205,2) &amp; "_g" &amp; TEXT(C205, "00") &amp; "_" &amp; TEXT(D205, "00") &amp; "_o" &amp; TEXT(E205, "00") &amp; IF(AND(ISNUMBER(F205), F205&lt;&gt;E205), "_" &amp; TEXT(F205, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C205),"arith_" &amp; INDEX(Operations[],J205,2) &amp; "_g" &amp; TEXT(C205, "00") &amp; "_" &amp; TEXT(D205, "00") &amp; "_o" &amp; TEXT(E205, "00") &amp; IF(AND(ISNUMBER(F205), F205&gt;E205), "_" &amp; TEXT(F205, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o05_06</v>
       </c>
       <c r="B205" t="str">
@@ -9012,7 +9022,7 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="str">
-        <f>IF(ISNUMBER(C206),"arith_" &amp; INDEX(Operations[],J206,2) &amp; "_g" &amp; TEXT(C206, "00") &amp; "_" &amp; TEXT(D206, "00") &amp; "_o" &amp; TEXT(E206, "00") &amp; IF(AND(ISNUMBER(F206), F206&lt;&gt;E206), "_" &amp; TEXT(F206, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C206),"arith_" &amp; INDEX(Operations[],J206,2) &amp; "_g" &amp; TEXT(C206, "00") &amp; "_" &amp; TEXT(D206, "00") &amp; "_o" &amp; TEXT(E206, "00") &amp; IF(AND(ISNUMBER(F206), F206&gt;E206), "_" &amp; TEXT(F206, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o06_07</v>
       </c>
       <c r="B206" t="str">
@@ -9054,7 +9064,7 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="str">
-        <f>IF(ISNUMBER(C207),"arith_" &amp; INDEX(Operations[],J207,2) &amp; "_g" &amp; TEXT(C207, "00") &amp; "_" &amp; TEXT(D207, "00") &amp; "_o" &amp; TEXT(E207, "00") &amp; IF(AND(ISNUMBER(F207), F207&lt;&gt;E207), "_" &amp; TEXT(F207, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C207),"arith_" &amp; INDEX(Operations[],J207,2) &amp; "_g" &amp; TEXT(C207, "00") &amp; "_" &amp; TEXT(D207, "00") &amp; "_o" &amp; TEXT(E207, "00") &amp; IF(AND(ISNUMBER(F207), F207&gt;E207), "_" &amp; TEXT(F207, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o07_08</v>
       </c>
       <c r="B207" t="str">
@@ -9096,7 +9106,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="str">
-        <f>IF(ISNUMBER(C208),"arith_" &amp; INDEX(Operations[],J208,2) &amp; "_g" &amp; TEXT(C208, "00") &amp; "_" &amp; TEXT(D208, "00") &amp; "_o" &amp; TEXT(E208, "00") &amp; IF(AND(ISNUMBER(F208), F208&lt;&gt;E208), "_" &amp; TEXT(F208, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C208),"arith_" &amp; INDEX(Operations[],J208,2) &amp; "_g" &amp; TEXT(C208, "00") &amp; "_" &amp; TEXT(D208, "00") &amp; "_o" &amp; TEXT(E208, "00") &amp; IF(AND(ISNUMBER(F208), F208&gt;E208), "_" &amp; TEXT(F208, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o08_09</v>
       </c>
       <c r="B208" t="str">
@@ -9138,7 +9148,7 @@
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" t="str">
-        <f>IF(ISNUMBER(C209),"arith_" &amp; INDEX(Operations[],J209,2) &amp; "_g" &amp; TEXT(C209, "00") &amp; "_" &amp; TEXT(D209, "00") &amp; "_o" &amp; TEXT(E209, "00") &amp; IF(AND(ISNUMBER(F209), F209&lt;&gt;E209), "_" &amp; TEXT(F209, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C209),"arith_" &amp; INDEX(Operations[],J209,2) &amp; "_g" &amp; TEXT(C209, "00") &amp; "_" &amp; TEXT(D209, "00") &amp; "_o" &amp; TEXT(E209, "00") &amp; IF(AND(ISNUMBER(F209), F209&gt;E209), "_" &amp; TEXT(F209, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o09_10</v>
       </c>
       <c r="B209" t="str">
@@ -9180,7 +9190,7 @@
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" t="str">
-        <f>IF(ISNUMBER(C210),"arith_" &amp; INDEX(Operations[],J210,2) &amp; "_g" &amp; TEXT(C210, "00") &amp; "_" &amp; TEXT(D210, "00") &amp; "_o" &amp; TEXT(E210, "00") &amp; IF(AND(ISNUMBER(F210), F210&lt;&gt;E210), "_" &amp; TEXT(F210, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C210),"arith_" &amp; INDEX(Operations[],J210,2) &amp; "_g" &amp; TEXT(C210, "00") &amp; "_" &amp; TEXT(D210, "00") &amp; "_o" &amp; TEXT(E210, "00") &amp; IF(AND(ISNUMBER(F210), F210&gt;E210), "_" &amp; TEXT(F210, "00"), ""), "")</f>
         <v>arith_sub_g09_00_o10</v>
       </c>
       <c r="B210" t="str">
@@ -9222,7 +9232,7 @@
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" t="str">
-        <f>IF(ISNUMBER(C211),"arith_" &amp; INDEX(Operations[],J211,2) &amp; "_g" &amp; TEXT(C211, "00") &amp; "_" &amp; TEXT(D211, "00") &amp; "_o" &amp; TEXT(E211, "00") &amp; IF(AND(ISNUMBER(F211), F211&lt;&gt;E211), "_" &amp; TEXT(F211, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C211),"arith_" &amp; INDEX(Operations[],J211,2) &amp; "_g" &amp; TEXT(C211, "00") &amp; "_" &amp; TEXT(D211, "00") &amp; "_o" &amp; TEXT(E211, "00") &amp; IF(AND(ISNUMBER(F211), F211&gt;E211), "_" &amp; TEXT(F211, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B211" t="str">
@@ -9264,7 +9274,7 @@
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" t="str">
-        <f>IF(ISNUMBER(C212),"arith_" &amp; INDEX(Operations[],J212,2) &amp; "_g" &amp; TEXT(C212, "00") &amp; "_" &amp; TEXT(D212, "00") &amp; "_o" &amp; TEXT(E212, "00") &amp; IF(AND(ISNUMBER(F212), F212&lt;&gt;E212), "_" &amp; TEXT(F212, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C212),"arith_" &amp; INDEX(Operations[],J212,2) &amp; "_g" &amp; TEXT(C212, "00") &amp; "_" &amp; TEXT(D212, "00") &amp; "_o" &amp; TEXT(E212, "00") &amp; IF(AND(ISNUMBER(F212), F212&gt;E212), "_" &amp; TEXT(F212, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o01_02</v>
       </c>
       <c r="B212" t="str">
@@ -9306,7 +9316,7 @@
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" t="str">
-        <f>IF(ISNUMBER(C213),"arith_" &amp; INDEX(Operations[],J213,2) &amp; "_g" &amp; TEXT(C213, "00") &amp; "_" &amp; TEXT(D213, "00") &amp; "_o" &amp; TEXT(E213, "00") &amp; IF(AND(ISNUMBER(F213), F213&lt;&gt;E213), "_" &amp; TEXT(F213, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C213),"arith_" &amp; INDEX(Operations[],J213,2) &amp; "_g" &amp; TEXT(C213, "00") &amp; "_" &amp; TEXT(D213, "00") &amp; "_o" &amp; TEXT(E213, "00") &amp; IF(AND(ISNUMBER(F213), F213&gt;E213), "_" &amp; TEXT(F213, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o02_03</v>
       </c>
       <c r="B213" t="str">
@@ -9348,7 +9358,7 @@
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" t="str">
-        <f>IF(ISNUMBER(C214),"arith_" &amp; INDEX(Operations[],J214,2) &amp; "_g" &amp; TEXT(C214, "00") &amp; "_" &amp; TEXT(D214, "00") &amp; "_o" &amp; TEXT(E214, "00") &amp; IF(AND(ISNUMBER(F214), F214&lt;&gt;E214), "_" &amp; TEXT(F214, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C214),"arith_" &amp; INDEX(Operations[],J214,2) &amp; "_g" &amp; TEXT(C214, "00") &amp; "_" &amp; TEXT(D214, "00") &amp; "_o" &amp; TEXT(E214, "00") &amp; IF(AND(ISNUMBER(F214), F214&gt;E214), "_" &amp; TEXT(F214, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o03_04</v>
       </c>
       <c r="B214" t="str">
@@ -9390,7 +9400,7 @@
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="str">
-        <f>IF(ISNUMBER(C215),"arith_" &amp; INDEX(Operations[],J215,2) &amp; "_g" &amp; TEXT(C215, "00") &amp; "_" &amp; TEXT(D215, "00") &amp; "_o" &amp; TEXT(E215, "00") &amp; IF(AND(ISNUMBER(F215), F215&lt;&gt;E215), "_" &amp; TEXT(F215, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C215),"arith_" &amp; INDEX(Operations[],J215,2) &amp; "_g" &amp; TEXT(C215, "00") &amp; "_" &amp; TEXT(D215, "00") &amp; "_o" &amp; TEXT(E215, "00") &amp; IF(AND(ISNUMBER(F215), F215&gt;E215), "_" &amp; TEXT(F215, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o04_05</v>
       </c>
       <c r="B215" t="str">
@@ -9432,7 +9442,7 @@
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" t="str">
-        <f>IF(ISNUMBER(C216),"arith_" &amp; INDEX(Operations[],J216,2) &amp; "_g" &amp; TEXT(C216, "00") &amp; "_" &amp; TEXT(D216, "00") &amp; "_o" &amp; TEXT(E216, "00") &amp; IF(AND(ISNUMBER(F216), F216&lt;&gt;E216), "_" &amp; TEXT(F216, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C216),"arith_" &amp; INDEX(Operations[],J216,2) &amp; "_g" &amp; TEXT(C216, "00") &amp; "_" &amp; TEXT(D216, "00") &amp; "_o" &amp; TEXT(E216, "00") &amp; IF(AND(ISNUMBER(F216), F216&gt;E216), "_" &amp; TEXT(F216, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o05_06</v>
       </c>
       <c r="B216" t="str">
@@ -9474,7 +9484,7 @@
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" t="str">
-        <f>IF(ISNUMBER(C217),"arith_" &amp; INDEX(Operations[],J217,2) &amp; "_g" &amp; TEXT(C217, "00") &amp; "_" &amp; TEXT(D217, "00") &amp; "_o" &amp; TEXT(E217, "00") &amp; IF(AND(ISNUMBER(F217), F217&lt;&gt;E217), "_" &amp; TEXT(F217, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C217),"arith_" &amp; INDEX(Operations[],J217,2) &amp; "_g" &amp; TEXT(C217, "00") &amp; "_" &amp; TEXT(D217, "00") &amp; "_o" &amp; TEXT(E217, "00") &amp; IF(AND(ISNUMBER(F217), F217&gt;E217), "_" &amp; TEXT(F217, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o06_07</v>
       </c>
       <c r="B217" t="str">
@@ -9516,7 +9526,7 @@
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" t="str">
-        <f>IF(ISNUMBER(C218),"arith_" &amp; INDEX(Operations[],J218,2) &amp; "_g" &amp; TEXT(C218, "00") &amp; "_" &amp; TEXT(D218, "00") &amp; "_o" &amp; TEXT(E218, "00") &amp; IF(AND(ISNUMBER(F218), F218&lt;&gt;E218), "_" &amp; TEXT(F218, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C218),"arith_" &amp; INDEX(Operations[],J218,2) &amp; "_g" &amp; TEXT(C218, "00") &amp; "_" &amp; TEXT(D218, "00") &amp; "_o" &amp; TEXT(E218, "00") &amp; IF(AND(ISNUMBER(F218), F218&gt;E218), "_" &amp; TEXT(F218, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o07_08</v>
       </c>
       <c r="B218" t="str">
@@ -9558,7 +9568,7 @@
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" t="str">
-        <f>IF(ISNUMBER(C219),"arith_" &amp; INDEX(Operations[],J219,2) &amp; "_g" &amp; TEXT(C219, "00") &amp; "_" &amp; TEXT(D219, "00") &amp; "_o" &amp; TEXT(E219, "00") &amp; IF(AND(ISNUMBER(F219), F219&lt;&gt;E219), "_" &amp; TEXT(F219, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C219),"arith_" &amp; INDEX(Operations[],J219,2) &amp; "_g" &amp; TEXT(C219, "00") &amp; "_" &amp; TEXT(D219, "00") &amp; "_o" &amp; TEXT(E219, "00") &amp; IF(AND(ISNUMBER(F219), F219&gt;E219), "_" &amp; TEXT(F219, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o08_09</v>
       </c>
       <c r="B219" t="str">
@@ -9600,7 +9610,7 @@
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="str">
-        <f>IF(ISNUMBER(C220),"arith_" &amp; INDEX(Operations[],J220,2) &amp; "_g" &amp; TEXT(C220, "00") &amp; "_" &amp; TEXT(D220, "00") &amp; "_o" &amp; TEXT(E220, "00") &amp; IF(AND(ISNUMBER(F220), F220&lt;&gt;E220), "_" &amp; TEXT(F220, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C220),"arith_" &amp; INDEX(Operations[],J220,2) &amp; "_g" &amp; TEXT(C220, "00") &amp; "_" &amp; TEXT(D220, "00") &amp; "_o" &amp; TEXT(E220, "00") &amp; IF(AND(ISNUMBER(F220), F220&gt;E220), "_" &amp; TEXT(F220, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o09_10</v>
       </c>
       <c r="B220" t="str">
@@ -9642,7 +9652,7 @@
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" t="str">
-        <f>IF(ISNUMBER(C221),"arith_" &amp; INDEX(Operations[],J221,2) &amp; "_g" &amp; TEXT(C221, "00") &amp; "_" &amp; TEXT(D221, "00") &amp; "_o" &amp; TEXT(E221, "00") &amp; IF(AND(ISNUMBER(F221), F221&lt;&gt;E221), "_" &amp; TEXT(F221, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C221),"arith_" &amp; INDEX(Operations[],J221,2) &amp; "_g" &amp; TEXT(C221, "00") &amp; "_" &amp; TEXT(D221, "00") &amp; "_o" &amp; TEXT(E221, "00") &amp; IF(AND(ISNUMBER(F221), F221&gt;E221), "_" &amp; TEXT(F221, "00"), ""), "")</f>
         <v>arith_sub_g10_00_o10</v>
       </c>
       <c r="B221" t="str">
@@ -9684,7 +9694,7 @@
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" t="str">
-        <f>IF(ISNUMBER(C222),"arith_" &amp; INDEX(Operations[],J222,2) &amp; "_g" &amp; TEXT(C222, "00") &amp; "_" &amp; TEXT(D222, "00") &amp; "_o" &amp; TEXT(E222, "00") &amp; IF(AND(ISNUMBER(F222), F222&lt;&gt;E222), "_" &amp; TEXT(F222, "00"), ""), "")</f>
+        <f>IF(ISNUMBER(C222),"arith_" &amp; INDEX(Operations[],J222,2) &amp; "_g" &amp; TEXT(C222, "00") &amp; "_" &amp; TEXT(D222, "00") &amp; "_o" &amp; TEXT(E222, "00") &amp; IF(AND(ISNUMBER(F222), F222&gt;E222), "_" &amp; TEXT(F222, "00"), ""), "")</f>
         <v/>
       </c>
       <c r="B222" t="str">
@@ -9729,7 +9739,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>_xlfn.ISFORMULA(A1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>